<commit_message>
Periodic check in - saving during drive crash fix
</commit_message>
<xml_diff>
--- a/documents/Features.xlsx
+++ b/documents/Features.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5542EA22-8D23-4282-910E-5F4F38264F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997DC2C5-C05A-4860-BB83-0DE980F8589A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Package pricing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
   <si>
     <t>Free</t>
   </si>
@@ -209,6 +208,15 @@
   </si>
   <si>
     <t>Can select multiples (15 or 30 minutes)</t>
+  </si>
+  <si>
+    <t>Billing Option</t>
+  </si>
+  <si>
+    <t>Team invitation</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -243,7 +251,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +306,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -471,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,6 +642,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -658,25 +693,18 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1002,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75CBC2-A4B4-4CDB-9F64-6654769FA256}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,91 +1258,129 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="42"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="C14" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="74"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="42"/>
-      <c r="C15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="8"/>
+      <c r="C15" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="78"/>
+      <c r="F15" s="75">
+        <v>10</v>
+      </c>
+      <c r="G15" s="75">
+        <v>50</v>
+      </c>
+      <c r="H15" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="74"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="42"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="30"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="42"/>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="42"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="42"/>
+      <c r="C19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F19" s="14">
         <v>1</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G19" s="14">
         <v>5</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="31" t="s">
+      <c r="I19" s="15"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="D16:I16"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="D14:I14"/>
     <mergeCell ref="D9:I9"/>
-    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="D4:I4"/>
-    <mergeCell ref="B6:B17"/>
+    <mergeCell ref="B6:B19"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1591,22 +1657,22 @@
     <row r="2" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="66" t="s">
+      <c r="E2" s="57"/>
+      <c r="F2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="66" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="66" t="s">
+      <c r="I2" s="57"/>
+      <c r="J2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="67"/>
+      <c r="K2" s="57"/>
       <c r="L2" s="21" t="s">
         <v>10</v>
       </c>
@@ -1643,30 +1709,30 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="58" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="71">
+      <c r="D4" s="61"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="61">
         <v>2</v>
       </c>
-      <c r="G4" s="72"/>
-      <c r="H4" s="71">
+      <c r="G4" s="62"/>
+      <c r="H4" s="61">
         <v>2</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="71">
+      <c r="I4" s="62"/>
+      <c r="J4" s="61">
         <v>1</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="62"/>
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1702,7 +1768,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
@@ -1738,7 +1804,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1774,7 +1840,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="69"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="3"/>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
@@ -1787,7 +1853,7 @@
       <c r="L8" s="39"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="69"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1822,7 +1888,7 @@
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="69"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
@@ -1857,7 +1923,7 @@
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="69"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1892,7 +1958,7 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
@@ -1927,7 +1993,7 @@
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="3"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -1940,7 +2006,7 @@
       <c r="L13" s="39"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="69"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
@@ -1975,7 +2041,7 @@
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="3"/>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
@@ -1988,7 +2054,7 @@
       <c r="L15" s="30"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="70"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="17" t="s">
         <v>21</v>
       </c>
@@ -2030,75 +2096,85 @@
         <v>113.77999999999999</v>
       </c>
       <c r="E18" s="40"/>
-      <c r="F18" s="56">
+      <c r="F18" s="63">
         <f>SUM(G5:G16)</f>
         <v>680.31</v>
       </c>
-      <c r="G18" s="57"/>
-      <c r="H18" s="56">
+      <c r="G18" s="64"/>
+      <c r="H18" s="63">
         <f>SUM(I5:I16)</f>
         <v>1789.18</v>
       </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="56">
+      <c r="I18" s="64"/>
+      <c r="J18" s="63">
         <f>SUM(K5:K16)</f>
         <v>3576.37</v>
       </c>
-      <c r="K18" s="57"/>
+      <c r="K18" s="64"/>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="61">
+      <c r="D19" s="68">
         <v>99.99</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="56">
+      <c r="E19" s="69"/>
+      <c r="F19" s="63">
         <v>699.99</v>
       </c>
-      <c r="G19" s="57"/>
-      <c r="H19" s="56">
+      <c r="G19" s="64"/>
+      <c r="H19" s="63">
         <v>1799.99</v>
       </c>
-      <c r="I19" s="57"/>
-      <c r="J19" s="56">
+      <c r="I19" s="64"/>
+      <c r="J19" s="63">
         <v>3599.99</v>
       </c>
-      <c r="K19" s="57"/>
+      <c r="K19" s="64"/>
       <c r="L19" s="8"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="63" t="s">
+      <c r="C21" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="65"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="72"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="60"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C22:L22"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C21:L21"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="D8:L8"/>
     <mergeCell ref="D13:L13"/>
@@ -2112,16 +2188,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C22:L22"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C21:L21"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#124.3 Preparation: changed client values to a record to include the client source (repo type)
</commit_message>
<xml_diff>
--- a/documents/Features.xlsx
+++ b/documents/Features.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997DC2C5-C05A-4860-BB83-0DE980F8589A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB59059-A37F-4443-8E0B-758DCD8CB472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="1" r:id="rId1"/>
     <sheet name="Prices" sheetId="2" r:id="rId2"/>
     <sheet name="Package pricing" sheetId="3" r:id="rId3"/>
+    <sheet name="Required sales" sheetId="4" r:id="rId4"/>
+    <sheet name="2003 Projections" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="98">
   <si>
     <t>Free</t>
   </si>
@@ -117,9 +119,6 @@
     <t>Number of log activities per day</t>
   </si>
   <si>
-    <t>1hr</t>
-  </si>
-  <si>
     <t>Time granularity</t>
   </si>
   <si>
@@ -138,9 +137,6 @@
     <t>Subitem</t>
   </si>
   <si>
-    <t>1 hour</t>
-  </si>
-  <si>
     <t>15 mins</t>
   </si>
   <si>
@@ -156,9 +152,6 @@
     <t>Truetime</t>
   </si>
   <si>
-    <t>An actual timestamp</t>
-  </si>
-  <si>
     <t>Pricing (monthly subscription)</t>
   </si>
   <si>
@@ -217,6 +210,156 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>1/2 hour</t>
+  </si>
+  <si>
+    <t>An actual timestamp right down to the second</t>
+  </si>
+  <si>
+    <t>Additional clients</t>
+  </si>
+  <si>
+    <t>Additional projects</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Hosting</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Salaries</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Potential Scenarios</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>1 min</t>
+  </si>
+  <si>
+    <t>GIT/JIRA accounts allowed</t>
+  </si>
+  <si>
+    <t>Total Revenue</t>
+  </si>
+  <si>
+    <t>Number of Sales Required</t>
+  </si>
+  <si>
+    <t>Estimated Release Date</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Try your own</t>
+  </si>
+  <si>
+    <t>First year projections (2023)</t>
+  </si>
+  <si>
+    <t>1st Quarter</t>
+  </si>
+  <si>
+    <t>Finish development</t>
+  </si>
+  <si>
+    <t>2nd Quarter</t>
+  </si>
+  <si>
+    <t>Number of Sales Required*</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>First year required monthly revenue for sustainability</t>
+  </si>
+  <si>
+    <t>Continued development</t>
+  </si>
+  <si>
+    <t>Beta testing (March only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA </t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Income*</t>
+  </si>
+  <si>
+    <t>Sales and marketing*</t>
+  </si>
+  <si>
+    <t>From sales</t>
+  </si>
+  <si>
+    <t>3rd Quarter</t>
+  </si>
+  <si>
+    <t>Monthly revenue</t>
+  </si>
+  <si>
+    <t>Additional Sales</t>
+  </si>
+  <si>
+    <t>4th Quarter</t>
+  </si>
+  <si>
+    <t>Sales commission</t>
+  </si>
+  <si>
+    <t>Total Income</t>
+  </si>
+  <si>
+    <t>Total Expenses</t>
+  </si>
+  <si>
+    <t>Second year projections (2024)+</t>
+  </si>
+  <si>
+    <t>*Sales projections are based on the target of profitability by the end of the year (2023). Monthly sales quotas are based on this figure
+divided by the number of active months from April, when the system is targetted to go live, to December when sales quotas will need to be reexamined.
+Sales is awarded a standard commission of 10% plus a base salary.
++Based on consistent sales from previous targets</t>
+  </si>
+  <si>
+    <t>Profit / Loss</t>
+  </si>
+  <si>
+    <t>Cumulative Profit / Loss</t>
+  </si>
+  <si>
+    <t>Third year projections (2025)+</t>
+  </si>
+  <si>
+    <t>Fourth year projections (2026)+</t>
   </si>
 </sst>
 </file>
@@ -227,7 +370,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,8 +393,16 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +460,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -527,7 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -558,146 +732,62 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,12 +796,243 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1032,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C75CBC2-A4B4-4CDB-9F64-6654769FA256}">
   <dimension ref="B2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,32 +1368,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="B2" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="41" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1093,7 +1414,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="45" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1119,7 +1440,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1143,7 +1464,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1163,21 +1484,21 @@
         <v>15</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1199,7 +1520,7 @@
       <c r="I10" s="8"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1212,16 +1533,16 @@
       <c r="F11" s="7">
         <v>20</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="40"/>
+      <c r="H11" s="43"/>
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
@@ -1232,14 +1553,14 @@
       <c r="F12" s="9">
         <v>100</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="40"/>
+      <c r="H12" s="43"/>
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1249,124 +1570,124 @@
       <c r="E13" s="7">
         <v>50</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="30"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="8"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="42"/>
-      <c r="C14" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="76" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="74"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="29"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
-      <c r="C15" s="73" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="75">
-        <v>10</v>
-      </c>
-      <c r="G15" s="75">
-        <v>50</v>
-      </c>
-      <c r="H15" s="75" t="s">
+      <c r="B15" s="45"/>
+      <c r="C15" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="49"/>
+      <c r="F15" s="30">
+        <v>5</v>
+      </c>
+      <c r="G15" s="30">
+        <v>25</v>
+      </c>
+      <c r="H15" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="74"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="45"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="45"/>
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="30"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="42"/>
-      <c r="C19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="14">
+      <c r="E19" s="27">
         <v>1</v>
       </c>
-      <c r="G19" s="14">
+      <c r="F19" s="31">
         <v>5</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="G19" s="33">
+        <v>25</v>
+      </c>
+      <c r="H19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="15"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="33"/>
+      <c r="C21" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="D18:I18"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="B2:I2"/>
@@ -1381,6 +1702,7 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1392,7 +1714,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D12" sqref="D12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,204 +1728,204 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="51"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="19" t="s">
-        <v>24</v>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="60">
         <v>9.99</v>
       </c>
-      <c r="E4" s="54"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="42"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="60">
         <v>5.99</v>
       </c>
-      <c r="E5" s="54"/>
+      <c r="E5" s="60"/>
       <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="60">
         <v>2.99</v>
       </c>
-      <c r="E6" s="54"/>
+      <c r="E6" s="60"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="42"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="30"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="45"/>
+      <c r="C8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="54">
-        <v>9.99</v>
-      </c>
-      <c r="E8" s="54"/>
+      <c r="D8" s="60">
+        <v>0.99</v>
+      </c>
+      <c r="E8" s="60"/>
       <c r="F8" s="12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="45"/>
+      <c r="C9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="54">
-        <v>1.99</v>
-      </c>
-      <c r="E9" s="54"/>
+      <c r="D9" s="60">
+        <v>0.99</v>
+      </c>
+      <c r="E9" s="60"/>
       <c r="F9" s="12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="54">
-        <v>0.99</v>
-      </c>
-      <c r="E10" s="54"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="60">
+        <v>0.49</v>
+      </c>
+      <c r="E10" s="60"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="42"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="45"/>
+      <c r="C11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="54">
-        <v>0.09</v>
-      </c>
-      <c r="E11" s="54"/>
+      <c r="D11" s="60">
+        <v>0.12</v>
+      </c>
+      <c r="E11" s="60"/>
       <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="42"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
-      <c r="C13" s="47" t="s">
-        <v>19</v>
+      <c r="B13" s="45"/>
+      <c r="C13" s="53" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="42"/>
-      <c r="C14" s="48"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" s="13">
         <v>2.99</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="42"/>
-      <c r="C15" s="48"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15" s="13">
         <v>5.99</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
-      <c r="C16" s="49"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="13">
         <v>9.99</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="42"/>
-      <c r="C18" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="54">
+      <c r="B18" s="45"/>
+      <c r="C18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="60">
         <v>4.99</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="60">
         <v>4.99</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1631,10 +1953,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1B9E85-2324-4849-9D4C-02218A174508}">
-  <dimension ref="B2:L22"/>
+  <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F19" sqref="F19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,123 +1965,123 @@
     <col min="2" max="2" width="3.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="26" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="26" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="27" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="26" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="27" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" style="26" customWidth="1"/>
     <col min="12" max="12" width="64.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="56" t="s">
+    <row r="2" spans="2:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="56" t="s">
+      <c r="E2" s="73"/>
+      <c r="F2" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="56" t="s">
+      <c r="G2" s="73"/>
+      <c r="H2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="56" t="s">
+      <c r="I2" s="73"/>
+      <c r="J2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="57"/>
-      <c r="L2" s="21" t="s">
+      <c r="K2" s="73"/>
+      <c r="L2" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="61">
+      <c r="C4" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="77">
         <v>2</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="61">
+      <c r="G4" s="78"/>
+      <c r="H4" s="77">
         <v>2</v>
       </c>
-      <c r="I4" s="62"/>
-      <c r="J4" s="61">
+      <c r="I4" s="78"/>
+      <c r="J4" s="77">
         <v>1</v>
       </c>
-      <c r="K4" s="62"/>
-      <c r="L4" s="25"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="24"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="59"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="14">
         <v>4</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <f>(F5-D5)*Prices!$D$4</f>
         <v>29.97</v>
       </c>
       <c r="H5" s="14">
         <v>9</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="22">
         <f>(H5-F5)*Prices!$D$4</f>
         <v>49.95</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="22">
         <f>2*I5/J$4</f>
         <v>99.9</v>
       </c>
@@ -1768,34 +2090,34 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="59"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="F6" s="14">
         <v>2</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="22">
         <f>F6*Prices!$D$4</f>
         <v>19.98</v>
       </c>
       <c r="H6" s="14">
         <v>5</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <f>(H6-F6)*Prices!$D$4</f>
         <v>29.97</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="22">
         <f>2*I6/J$4</f>
         <v>59.94</v>
       </c>
@@ -1804,284 +2126,284 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="59"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="F7" s="14">
         <v>5</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <f>F7*Prices!$D$4</f>
         <v>49.95</v>
       </c>
       <c r="H7" s="14">
         <v>25</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="22">
         <f>(H7-F7)*Prices!$D$4</f>
         <v>199.8</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="22">
         <f>2*I7/J$4</f>
         <v>399.6</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="59"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="59"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <f>D9*Prices!D8</f>
-        <v>39.96</v>
+        <v>3.96</v>
       </c>
       <c r="F9" s="14">
         <v>9</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="22">
         <f>((F9-D9)*Prices!$D$4)/$F$4</f>
         <v>24.975000000000001</v>
       </c>
       <c r="H9" s="14">
         <v>49</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <f>(H9-F9)*Prices!$D$4</f>
         <v>399.6</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="22">
         <f>2*I9/J$4</f>
         <v>799.2</v>
       </c>
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="59"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="D10" s="7">
         <v>9</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <f>D10*Prices!D9</f>
-        <v>17.91</v>
+        <v>8.91</v>
       </c>
       <c r="F10" s="14">
         <v>19</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="22">
         <f>((F10-D10)*Prices!$D$4)/$F$4</f>
         <v>49.95</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="22">
         <f>(F10*Prices!$D$4)/H$4</f>
         <v>94.905000000000001</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="22">
         <f>2*I10/J$4</f>
         <v>189.81</v>
       </c>
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="59"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7">
         <v>49</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <f>D11*Prices!D10</f>
-        <v>48.51</v>
+        <v>24.009999999999998</v>
       </c>
       <c r="F11" s="14">
         <v>99</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="22">
         <f>((F11-D11)*Prices!$D$4)/$F$4</f>
         <v>249.75</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="22">
         <f>(F11*Prices!$D$4)/H$4</f>
         <v>494.505</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="22">
         <f>2*I11/J$4</f>
         <v>989.01</v>
       </c>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="59"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="7">
         <v>49</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <f>D12*Prices!D11</f>
-        <v>4.41</v>
+        <v>5.88</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <f>(D12*Prices!$D$4)/F$4</f>
         <v>244.755</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="22">
         <f>(D12*Prices!$D$4*2)/H$4</f>
         <v>489.51</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="22">
         <f>2*I12/J$4</f>
         <v>979.02</v>
       </c>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="59"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="39"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="42"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="59"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="22">
+        <v>34</v>
+      </c>
+      <c r="E14" s="21">
         <f>Prices!E14</f>
         <v>2.99</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="23">
+        <v>35</v>
+      </c>
+      <c r="G14" s="22">
         <f>Prices!$E$15</f>
         <v>5.99</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="23">
+        <v>35</v>
+      </c>
+      <c r="I14" s="22">
         <f>Prices!$E$15</f>
         <v>5.99</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="23">
+        <v>28</v>
+      </c>
+      <c r="K14" s="22">
         <f>Prices!$E$16</f>
         <v>9.99</v>
       </c>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="59"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="30"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="60"/>
-      <c r="C16" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>40</v>
+      <c r="B16" s="76"/>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="27">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21">
+        <v>4.99</v>
       </c>
       <c r="F16" s="14">
         <v>1</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="22">
         <f>F16*Prices!$D$18</f>
         <v>4.99</v>
       </c>
       <c r="H16" s="14">
         <v>5</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="22">
         <f>H16*Prices!$D$18</f>
         <v>24.950000000000003</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="22">
         <f>2*I16/J$4</f>
         <v>49.900000000000006</v>
       </c>
@@ -2089,92 +2411,108 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="54">
-        <f>SUM(E9:E12,E14)</f>
-        <v>113.77999999999999</v>
-      </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="63">
+        <v>40</v>
+      </c>
+      <c r="D18" s="60">
+        <f>SUM(E9:E12,E14,E16)</f>
+        <v>50.74</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="F18" s="62">
         <f>SUM(G5:G16)</f>
         <v>680.31</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="63">
+      <c r="G18" s="63"/>
+      <c r="H18" s="62">
         <f>SUM(I5:I16)</f>
         <v>1789.18</v>
       </c>
-      <c r="I18" s="64"/>
-      <c r="J18" s="63">
+      <c r="I18" s="63"/>
+      <c r="J18" s="62">
         <f>SUM(K5:K16)</f>
         <v>3576.37</v>
       </c>
-      <c r="K18" s="64"/>
+      <c r="K18" s="63"/>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="68">
-        <v>99.99</v>
-      </c>
-      <c r="E19" s="69"/>
-      <c r="F19" s="63">
-        <v>699.99</v>
-      </c>
-      <c r="G19" s="64"/>
-      <c r="H19" s="63">
-        <v>1799.99</v>
-      </c>
-      <c r="I19" s="64"/>
-      <c r="J19" s="63">
-        <v>3599.99</v>
-      </c>
-      <c r="K19" s="64"/>
+        <v>43</v>
+      </c>
+      <c r="D19" s="67">
+        <v>49.99</v>
+      </c>
+      <c r="E19" s="68"/>
+      <c r="F19" s="62">
+        <v>599.99</v>
+      </c>
+      <c r="G19" s="63"/>
+      <c r="H19" s="62">
+        <v>1499.99</v>
+      </c>
+      <c r="I19" s="63"/>
+      <c r="J19" s="62">
+        <v>2799.99</v>
+      </c>
+      <c r="K19" s="63"/>
       <c r="L19" s="8"/>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="70" t="s">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="79">
+        <f>(D19/D18)</f>
+        <v>0.98521876231769812</v>
+      </c>
+      <c r="E20" s="80"/>
+      <c r="F20" s="79">
+        <f>(F19/F18)</f>
+        <v>0.88193617615498821</v>
+      </c>
+      <c r="G20" s="80"/>
+      <c r="H20" s="79">
+        <f>(H19/H18)</f>
+        <v>0.83836729675046662</v>
+      </c>
+      <c r="I20" s="80"/>
+      <c r="J20" s="79">
+        <f>(J19/J18)</f>
+        <v>0.78291396024460558</v>
+      </c>
+      <c r="K20" s="80"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="71"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C23" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="72"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="67"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="65"/>
+      <c r="L23" s="66"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C22:L22"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="C21:L21"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
+  <mergeCells count="27">
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="D8:L8"/>
     <mergeCell ref="D13:L13"/>
@@ -2188,8 +2526,1660 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C23:L23"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="C22:L22"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB03894-93D0-495C-B3BA-C4E55DD6402D}">
+  <dimension ref="B2:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="81" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="81" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="105">
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="106">
+        <v>7916.666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="94"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="106">
+        <v>3333.3333333333298</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="94"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="106">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="94"/>
+      <c r="C8" s="99" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="100"/>
+      <c r="E8" s="106">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="94"/>
+      <c r="C9" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="100"/>
+      <c r="E9" s="106">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="95"/>
+      <c r="C10" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="100"/>
+      <c r="E10" s="106">
+        <v>1671.9999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="96"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="107">
+        <f>SUM(E5:E10)</f>
+        <v>16871.999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="90" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="91"/>
+      <c r="J14" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="82">
+        <v>338</v>
+      </c>
+      <c r="C15" s="84">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D15" s="82">
+        <v>0</v>
+      </c>
+      <c r="E15" s="84">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F15" s="83">
+        <v>0</v>
+      </c>
+      <c r="G15" s="84">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H15" s="83">
+        <v>0</v>
+      </c>
+      <c r="I15" s="84">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J15" s="84">
+        <f>SUM((B15*C15),(D15*E15),(F15*G15),(H15*I15))</f>
+        <v>16896.62</v>
+      </c>
+      <c r="K15" s="97">
+        <f>SUM(B15,D15,F15,H15)</f>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="82">
+        <v>0</v>
+      </c>
+      <c r="C16" s="84">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D16" s="82">
+        <v>29</v>
+      </c>
+      <c r="E16" s="84">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F16" s="83">
+        <v>0</v>
+      </c>
+      <c r="G16" s="84">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H16" s="83">
+        <v>0</v>
+      </c>
+      <c r="I16" s="84">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J16" s="84">
+        <f>SUM((B16*C16),(D16*E16),(F16*G16),(H16*I16))</f>
+        <v>17399.71</v>
+      </c>
+      <c r="K16" s="97">
+        <f t="shared" ref="K16:K18" si="0">SUM(B16,D16,F16,H16)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="82">
+        <v>0</v>
+      </c>
+      <c r="C17" s="84">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D17" s="82">
+        <v>0</v>
+      </c>
+      <c r="E17" s="84">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F17" s="83">
+        <v>12</v>
+      </c>
+      <c r="G17" s="84">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H17" s="83">
+        <v>0</v>
+      </c>
+      <c r="I17" s="84">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J17" s="84">
+        <f>SUM((B17*C17),(D17*E17),(F17*G17),(H17*I17))</f>
+        <v>17999.88</v>
+      </c>
+      <c r="K17" s="97">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="82">
+        <v>0</v>
+      </c>
+      <c r="C18" s="84">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D18" s="82">
+        <v>0</v>
+      </c>
+      <c r="E18" s="84">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F18" s="83">
+        <v>0</v>
+      </c>
+      <c r="G18" s="84">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H18" s="83">
+        <v>7</v>
+      </c>
+      <c r="I18" s="84">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J18" s="84">
+        <f>SUM((B18*C18),(D18*E18),(F18*G18),(H18*I18))</f>
+        <v>19599.93</v>
+      </c>
+      <c r="K18" s="97">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="90" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="91"/>
+      <c r="J21" s="92" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" s="92" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="82">
+        <v>0</v>
+      </c>
+      <c r="C22" s="84">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D22" s="82">
+        <v>0</v>
+      </c>
+      <c r="E22" s="84">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F22" s="83">
+        <v>0</v>
+      </c>
+      <c r="G22" s="84">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H22" s="83">
+        <v>0</v>
+      </c>
+      <c r="I22" s="84">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J22" s="84">
+        <f>SUM((B22*C22),(D22*E22),(F22*G22),(H22*I22))</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="97">
+        <f>SUM(B22,D22,F22,H22)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F647B2FF-201C-44DE-9C82-A6B59556EC9F}">
+  <dimension ref="B2:P43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="108" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="89"/>
+      <c r="F2" s="87" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="88"/>
+      <c r="H2" s="89"/>
+      <c r="J2" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="88"/>
+      <c r="L2" s="89"/>
+      <c r="N2" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" s="88"/>
+      <c r="P2" s="89"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="112"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="117" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="96"/>
+      <c r="F4" s="117" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="96"/>
+      <c r="J4" s="117" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="96"/>
+      <c r="N4" s="117" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="96"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="117"/>
+      <c r="C5" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="F5" s="117"/>
+      <c r="G5" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="J5" s="117"/>
+      <c r="K5" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="N5" s="117"/>
+      <c r="O5" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="117"/>
+      <c r="C6" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="109">
+        <f>40000/12</f>
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="F6" s="117"/>
+      <c r="G6" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="109">
+        <f>40000/12</f>
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="J6" s="117"/>
+      <c r="K6" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="109">
+        <f>40000/12</f>
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="N6" s="117"/>
+      <c r="O6" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="109">
+        <f>40000/12</f>
+        <v>3333.3333333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="117"/>
+      <c r="C7" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="122" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="117"/>
+      <c r="G7" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="109">
+        <f>12500+(H10*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="J7" s="117"/>
+      <c r="K7" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="109">
+        <f>12500+(L10*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="N7" s="117"/>
+      <c r="O7" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" s="109">
+        <f>12500+(P10*0.1)</f>
+        <v>13062.4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="117"/>
+      <c r="C8" s="96" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="96"/>
+      <c r="F8" s="117"/>
+      <c r="G8" s="96" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="96"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="96" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="96"/>
+      <c r="N8" s="117"/>
+      <c r="O8" s="96" t="s">
+        <v>80</v>
+      </c>
+      <c r="P8" s="96"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="117"/>
+      <c r="C9" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="120" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="117"/>
+      <c r="G9" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="109">
+        <f>SUM(D33+D34)</f>
+        <v>16871.999999999996</v>
+      </c>
+      <c r="J9" s="117"/>
+      <c r="K9" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="109">
+        <f>SUM(H33+H34)</f>
+        <v>39367.999999999993</v>
+      </c>
+      <c r="N9" s="117"/>
+      <c r="O9" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="P9" s="109">
+        <f>SUM(L33+L34)</f>
+        <v>61863.999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="117"/>
+      <c r="C10" s="121" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="120" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="117"/>
+      <c r="G10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="J10" s="117"/>
+      <c r="K10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="N10" s="117"/>
+      <c r="O10" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="P10" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="113"/>
+      <c r="C11" s="114"/>
+      <c r="D11" s="115"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="115"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="114"/>
+      <c r="L11" s="115"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="114"/>
+      <c r="P11" s="115"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="96"/>
+      <c r="F12" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="96"/>
+      <c r="J12" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="L12" s="96"/>
+      <c r="N12" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="96"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="94"/>
+      <c r="C13" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="F13" s="94"/>
+      <c r="G13" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="J13" s="94"/>
+      <c r="K13" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="N13" s="94"/>
+      <c r="O13" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="P13" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="94"/>
+      <c r="C14" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="109">
+        <v>10000</v>
+      </c>
+      <c r="F14" s="94"/>
+      <c r="G14" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="109">
+        <v>10000</v>
+      </c>
+      <c r="J14" s="94"/>
+      <c r="K14" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="L14" s="109">
+        <v>10000</v>
+      </c>
+      <c r="N14" s="94"/>
+      <c r="O14" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="P14" s="109">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="94"/>
+      <c r="C15" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="109">
+        <f>12500+(D18*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="F15" s="94"/>
+      <c r="G15" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="109">
+        <f>12500+(H18*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="J15" s="94"/>
+      <c r="K15" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="109">
+        <f>12500+(L18*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="N15" s="94"/>
+      <c r="O15" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="P15" s="109">
+        <f>12500+(P18*0.1)</f>
+        <v>13062.4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="94"/>
+      <c r="C16" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="96"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="96"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" s="96"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="P16" s="96"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="94"/>
+      <c r="C17" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="120" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="94"/>
+      <c r="G17" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="123">
+        <f>SUM(H9:H10)</f>
+        <v>22495.999999999996</v>
+      </c>
+      <c r="J17" s="94"/>
+      <c r="K17" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="123">
+        <f>SUM(L9:L10)</f>
+        <v>44991.999999999993</v>
+      </c>
+      <c r="N17" s="94"/>
+      <c r="O17" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="P17" s="123">
+        <f>SUM(P9:P10)</f>
+        <v>67487.999999999985</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="95"/>
+      <c r="C18" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="F18" s="95"/>
+      <c r="G18" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="J18" s="95"/>
+      <c r="K18" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="N18" s="95"/>
+      <c r="O18" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="P18" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H19" s="108"/>
+      <c r="L19" s="108"/>
+      <c r="P19" s="108"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="118" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="96"/>
+      <c r="F20" s="118" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="96"/>
+      <c r="J20" s="118" t="s">
+        <v>85</v>
+      </c>
+      <c r="K20" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="L20" s="96"/>
+      <c r="N20" s="118" t="s">
+        <v>85</v>
+      </c>
+      <c r="O20" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="P20" s="96"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="118"/>
+      <c r="C21" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="F21" s="118"/>
+      <c r="G21" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="J21" s="118"/>
+      <c r="K21" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="L21" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="N21" s="118"/>
+      <c r="O21" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="P21" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="118"/>
+      <c r="C22" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="109">
+        <v>10000</v>
+      </c>
+      <c r="F22" s="118"/>
+      <c r="G22" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="109">
+        <v>10000</v>
+      </c>
+      <c r="J22" s="118"/>
+      <c r="K22" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" s="109">
+        <v>10000</v>
+      </c>
+      <c r="N22" s="118"/>
+      <c r="O22" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="P22" s="109">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="118"/>
+      <c r="C23" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="109">
+        <f>12500+(D25*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="F23" s="118"/>
+      <c r="G23" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="109">
+        <f>12500+(H26*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="J23" s="118"/>
+      <c r="K23" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="L23" s="109">
+        <f>12500+(L26*0.1)</f>
+        <v>13062.4</v>
+      </c>
+      <c r="N23" s="118"/>
+      <c r="O23" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="P23" s="109">
+        <f>12500+(P26*0.1)</f>
+        <v>13062.4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="118"/>
+      <c r="C24" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="96"/>
+      <c r="F24" s="118"/>
+      <c r="G24" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" s="96"/>
+      <c r="J24" s="118"/>
+      <c r="K24" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="L24" s="96"/>
+      <c r="N24" s="118"/>
+      <c r="O24" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="P24" s="96"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25" s="118"/>
+      <c r="C25" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="109">
+        <f>D18</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="F25" s="118"/>
+      <c r="G25" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="109">
+        <f>SUM(H17:H18)</f>
+        <v>28119.999999999996</v>
+      </c>
+      <c r="J25" s="118"/>
+      <c r="K25" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="L25" s="109">
+        <f>SUM(L17:L18)</f>
+        <v>50615.999999999993</v>
+      </c>
+      <c r="N25" s="118"/>
+      <c r="O25" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="P25" s="109">
+        <f>SUM(P17:P18)</f>
+        <v>73111.999999999985</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26" s="118"/>
+      <c r="C26" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="F26" s="118"/>
+      <c r="G26" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="J26" s="118"/>
+      <c r="K26" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="L26" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="N26" s="118"/>
+      <c r="O26" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="P26" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H27" s="108"/>
+      <c r="L27" s="108"/>
+      <c r="P27" s="108"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="118" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="96"/>
+      <c r="F28" s="118" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="H28" s="96"/>
+      <c r="J28" s="118" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" s="96"/>
+      <c r="N28" s="118" t="s">
+        <v>88</v>
+      </c>
+      <c r="O28" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="P28" s="96"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="118"/>
+      <c r="C29" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="F29" s="118"/>
+      <c r="G29" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="J29" s="118"/>
+      <c r="K29" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="L29" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+      <c r="N29" s="118"/>
+      <c r="O29" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="P29" s="109">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="118"/>
+      <c r="C30" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="109">
+        <v>10000</v>
+      </c>
+      <c r="F30" s="118"/>
+      <c r="G30" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="109">
+        <v>10000</v>
+      </c>
+      <c r="J30" s="118"/>
+      <c r="K30" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="L30" s="109">
+        <v>10000</v>
+      </c>
+      <c r="N30" s="118"/>
+      <c r="O30" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="P30" s="109">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="118"/>
+      <c r="C31" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="109">
+        <f>12500+(D33*0.1)</f>
+        <v>13624.8</v>
+      </c>
+      <c r="F31" s="118"/>
+      <c r="G31" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" s="109">
+        <f>12500+(H33*0.1)</f>
+        <v>15874.4</v>
+      </c>
+      <c r="J31" s="118"/>
+      <c r="K31" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="L31" s="109">
+        <f>12500+(L33*0.1)</f>
+        <v>18124</v>
+      </c>
+      <c r="N31" s="118"/>
+      <c r="O31" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="P31" s="109">
+        <f>12500+(P33*0.1)</f>
+        <v>20373.599999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="118"/>
+      <c r="C32" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="96"/>
+      <c r="F32" s="118"/>
+      <c r="G32" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="96"/>
+      <c r="J32" s="118"/>
+      <c r="K32" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="L32" s="96"/>
+      <c r="N32" s="118"/>
+      <c r="O32" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="P32" s="96"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="118"/>
+      <c r="C33" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="109">
+        <f>D25+D26</f>
+        <v>11247.999999999998</v>
+      </c>
+      <c r="F33" s="118"/>
+      <c r="G33" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="109">
+        <f>H25+H26</f>
+        <v>33743.999999999993</v>
+      </c>
+      <c r="J33" s="118"/>
+      <c r="K33" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="L33" s="109">
+        <f>L25+L26</f>
+        <v>56239.999999999993</v>
+      </c>
+      <c r="N33" s="118"/>
+      <c r="O33" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="P33" s="109">
+        <f>P25+P26</f>
+        <v>78735.999999999985</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="118"/>
+      <c r="C34" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="F34" s="118"/>
+      <c r="G34" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="H34" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="J34" s="118"/>
+      <c r="K34" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="L34" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+      <c r="N34" s="118"/>
+      <c r="O34" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="P34" s="109">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H35" s="108"/>
+      <c r="L35" s="108"/>
+      <c r="P35" s="108"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B36" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="110"/>
+      <c r="D36" s="109">
+        <f>SUM(D18,D25:D26,D33:D34)</f>
+        <v>33743.999999999993</v>
+      </c>
+      <c r="F36" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="110"/>
+      <c r="H36" s="109">
+        <f>SUM(H9:H10,H17:H18,H25:H26,H33:H34)</f>
+        <v>123727.99999999997</v>
+      </c>
+      <c r="J36" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="K36" s="110"/>
+      <c r="L36" s="109">
+        <f>SUM(L9:L10,L17:L18,L25:L26,L33:L34)</f>
+        <v>213711.99999999997</v>
+      </c>
+      <c r="N36" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="O36" s="110"/>
+      <c r="P36" s="109">
+        <f>SUM(P9:P10,P17:P18,P25:P26,P33:P34)</f>
+        <v>303695.99999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="110"/>
+      <c r="D37" s="109">
+        <f>SUM(D5:D6,D13:D15,D21:D23,D29:D31)</f>
+        <v>168082.93333333329</v>
+      </c>
+      <c r="F37" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="110"/>
+      <c r="H37" s="109">
+        <f>SUM(H5:H6,H13:H15,H21:H23,H29:H31)</f>
+        <v>170332.5333333333</v>
+      </c>
+      <c r="J37" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="K37" s="110"/>
+      <c r="L37" s="109">
+        <f>SUM(L5:L6,L13:L15,L21:L23,L29:L31)</f>
+        <v>172582.1333333333</v>
+      </c>
+      <c r="N37" s="110" t="s">
+        <v>91</v>
+      </c>
+      <c r="O37" s="110"/>
+      <c r="P37" s="109">
+        <f>SUM(P5:P6,P13:P15,P21:P23,P29:P31)</f>
+        <v>174831.73333333331</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H38" s="108"/>
+      <c r="L38" s="108"/>
+      <c r="P38" s="108"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="98"/>
+      <c r="D39" s="109">
+        <f>D37-D36</f>
+        <v>134338.93333333329</v>
+      </c>
+      <c r="F39" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="98"/>
+      <c r="H39" s="109">
+        <f>H37-H36</f>
+        <v>46604.533333333326</v>
+      </c>
+      <c r="J39" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="K39" s="98"/>
+      <c r="L39" s="109">
+        <f>L37-L36</f>
+        <v>-41129.866666666669</v>
+      </c>
+      <c r="N39" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="O39" s="98"/>
+      <c r="P39" s="109">
+        <f>P37-P36</f>
+        <v>-128864.26666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="98" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="98"/>
+      <c r="D40" s="109">
+        <f>D39</f>
+        <v>134338.93333333329</v>
+      </c>
+      <c r="F40" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="G40" s="98"/>
+      <c r="H40" s="109">
+        <f>D40+H39</f>
+        <v>180943.46666666662</v>
+      </c>
+      <c r="J40" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="K40" s="98"/>
+      <c r="L40" s="109">
+        <f>H40+L39</f>
+        <v>139813.59999999995</v>
+      </c>
+      <c r="N40" s="98" t="s">
+        <v>94</v>
+      </c>
+      <c r="O40" s="98"/>
+      <c r="P40" s="109">
+        <f>L40+P39</f>
+        <v>10949.333333333314</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" s="98" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="98"/>
+      <c r="D42" s="98"/>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="98"/>
+      <c r="I42" s="98"/>
+      <c r="J42" s="98"/>
+      <c r="K42" s="98"/>
+    </row>
+    <row r="43" spans="2:16" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="116" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="102"/>
+      <c r="D43" s="102"/>
+      <c r="E43" s="102"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="102"/>
+      <c r="I43" s="102"/>
+      <c r="J43" s="102"/>
+      <c r="K43" s="102"/>
+    </row>
+  </sheetData>
+  <mergeCells count="70">
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N20:N26"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="N28:N34"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N4:N10"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="N12:N18"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="J20:J26"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="J28:J34"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="F4:F10"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="J12:J18"/>
+    <mergeCell ref="F20:F26"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="F28:F34"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="F12:F18"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C8:D8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D39:D40">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L39:L40 H39:H40">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P39:P40">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#124.3 Preparation including using a record for the client selector instead of just an id (includes repo type)
</commit_message>
<xml_diff>
--- a/documents/Features.xlsx
+++ b/documents/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB59059-A37F-4443-8E0B-758DCD8CB472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E7610D-CD25-4630-BF31-E97520E0B87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
   </bookViews>
@@ -987,7 +987,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1013,12 +1035,18 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="-0.24994659260841701"/>
+        <strike val="0"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -1032,10 +1060,16 @@
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF008000"/>
       <color rgb="FFEEE8E4"/>
       <color rgb="FFA66642"/>
       <color rgb="FFF2E6E0"/>
@@ -2955,8 +2989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F647B2FF-201C-44DE-9C82-A6B59556EC9F}">
   <dimension ref="B2:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,16 +4027,16 @@
       </c>
       <c r="C39" s="98"/>
       <c r="D39" s="109">
-        <f>D37-D36</f>
-        <v>134338.93333333329</v>
+        <f>0-(D37-D36)</f>
+        <v>-134338.93333333329</v>
       </c>
       <c r="F39" s="98" t="s">
         <v>94</v>
       </c>
       <c r="G39" s="98"/>
       <c r="H39" s="109">
-        <f>H37-H36</f>
-        <v>46604.533333333326</v>
+        <f>0-(H37-H36)</f>
+        <v>-46604.533333333326</v>
       </c>
       <c r="J39" s="98" t="s">
         <v>94</v>
@@ -4028,14 +4062,14 @@
       <c r="C40" s="98"/>
       <c r="D40" s="109">
         <f>D39</f>
-        <v>134338.93333333329</v>
+        <v>-134338.93333333329</v>
       </c>
       <c r="F40" s="98" t="s">
         <v>94</v>
       </c>
       <c r="G40" s="98"/>
       <c r="H40" s="109">
-        <f>D40+H39</f>
+        <f>0-(D40+H39)</f>
         <v>180943.46666666662</v>
       </c>
       <c r="J40" s="98" t="s">
@@ -4157,26 +4191,26 @@
     <mergeCell ref="C8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="D39:D40">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:L40 H39:H40">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P39:P40">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#128 - Added calendar clock option to the logging page. Added start time with link on log. Administrative: Updated Features document with sales return estimates.
</commit_message>
<xml_diff>
--- a/documents/Features.xlsx
+++ b/documents/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E7610D-CD25-4630-BF31-E97520E0B87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872C793D-8BEC-496E-AC08-41401240F406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="103">
   <si>
     <t>Free</t>
   </si>
@@ -239,9 +239,6 @@
     <t>Development</t>
   </si>
   <si>
-    <t>Potential Scenarios</t>
-  </si>
-  <si>
     <t>Company</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>Total Revenue</t>
   </si>
   <si>
-    <t>Number of Sales Required</t>
-  </si>
-  <si>
     <t>Estimated Release Date</t>
   </si>
   <si>
@@ -284,9 +278,6 @@
     <t>2nd Quarter</t>
   </si>
   <si>
-    <t>Number of Sales Required*</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -344,22 +335,46 @@
     <t>Second year projections (2024)+</t>
   </si>
   <si>
+    <t>Profit / Loss</t>
+  </si>
+  <si>
+    <t>Cumulative Profit / Loss</t>
+  </si>
+  <si>
+    <t>Third year projections (2025)+</t>
+  </si>
+  <si>
+    <t>Fourth year projections (2026)+</t>
+  </si>
+  <si>
+    <t>Fifth year projections (2027)+</t>
+  </si>
+  <si>
     <t>*Sales projections are based on the target of profitability by the end of the year (2023). Monthly sales quotas are based on this figure
-divided by the number of active months from April, when the system is targetted to go live, to December when sales quotas will need to be reexamined.
+divided by the number of active months from April, when the system is targetted to go live, to December when sales quotas will need to be reexamined (9 months).
 Sales is awarded a standard commission of 10% plus a base salary.
 +Based on consistent sales from previous targets</t>
   </si>
   <si>
-    <t>Profit / Loss</t>
-  </si>
-  <si>
-    <t>Cumulative Profit / Loss</t>
-  </si>
-  <si>
-    <t>Third year projections (2025)+</t>
-  </si>
-  <si>
-    <t>Fourth year projections (2026)+</t>
+    <t>Subscriptions required for each category</t>
+  </si>
+  <si>
+    <t>Subscriptions*</t>
+  </si>
+  <si>
+    <t>Sales*</t>
+  </si>
+  <si>
+    <t>Total sales</t>
+  </si>
+  <si>
+    <t>Monthly sales target</t>
+  </si>
+  <si>
+    <t>Total monthly break-even revenue</t>
+  </si>
+  <si>
+    <t>Monthly new sales required for each category</t>
   </si>
 </sst>
 </file>
@@ -660,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -738,156 +753,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -896,62 +761,14 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -961,15 +778,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -982,6 +790,225 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -991,44 +1018,33 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="-0.24994659260841701"/>
+        <strike val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <strike val="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF008000"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
@@ -1063,6 +1079,17 @@
     <dxf>
       <font>
         <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color rgb="FF008000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
   </dxfs>
@@ -1402,32 +1429,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="39"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="63"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="44" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1475,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="69" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1474,7 +1501,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1498,7 +1525,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1522,17 +1549,17 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="42"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="66"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1581,7 @@
       <c r="I10" s="8"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1567,14 +1594,14 @@
       <c r="F11" s="7">
         <v>20</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="43"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1587,14 +1614,14 @@
       <c r="F12" s="9">
         <v>100</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="43"/>
+      <c r="H12" s="67"/>
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1604,38 +1631,38 @@
       <c r="E13" s="7">
         <v>50</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
       <c r="I13" s="8"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="45"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="28" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="45"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="49"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="30">
         <v>5</v>
       </c>
@@ -1648,49 +1675,49 @@
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="45"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="66"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="45"/>
+      <c r="B17" s="69"/>
       <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="33"/>
+      <c r="F17" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="57"/>
       <c r="H17" s="7" t="s">
         <v>28</v>
       </c>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="45"/>
+      <c r="B18" s="69"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="57"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="45"/>
+      <c r="B19" s="69"/>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>19</v>
@@ -1698,10 +1725,10 @@
       <c r="E19" s="27">
         <v>1</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="55">
         <v>5</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="57">
         <v>25</v>
       </c>
       <c r="H19" s="27" t="s">
@@ -1710,15 +1737,15 @@
       <c r="I19" s="8"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="36"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1762,17 +1789,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="50" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="52"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="76"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1784,111 +1811,111 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="69" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="60">
+      <c r="D4" s="84">
         <v>9.99</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="84"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="45"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="84">
         <v>5.99</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="84"/>
       <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="45"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="84">
         <v>2.99</v>
       </c>
-      <c r="E6" s="60"/>
+      <c r="E6" s="84"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="33"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="84">
         <v>0.99</v>
       </c>
-      <c r="E8" s="60"/>
+      <c r="E8" s="84"/>
       <c r="F8" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="45"/>
+      <c r="B9" s="69"/>
       <c r="C9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="84">
         <v>0.99</v>
       </c>
-      <c r="E9" s="60"/>
+      <c r="E9" s="84"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="84">
         <v>0.49</v>
       </c>
-      <c r="E10" s="60"/>
+      <c r="E10" s="84"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="45"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="84">
         <v>0.12</v>
       </c>
-      <c r="E11" s="60"/>
+      <c r="E11" s="84"/>
       <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="45"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="45"/>
-      <c r="C13" s="53" t="s">
+      <c r="B13" s="69"/>
+      <c r="C13" s="77" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1902,8 +1929,8 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="45"/>
-      <c r="C14" s="54"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="7" t="s">
         <v>24</v>
       </c>
@@ -1915,8 +1942,8 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="45"/>
-      <c r="C15" s="54"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="7" t="s">
         <v>25</v>
       </c>
@@ -1928,8 +1955,8 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="45"/>
-      <c r="C16" s="55"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="79"/>
       <c r="D16" s="7" t="s">
         <v>28</v>
       </c>
@@ -1941,21 +1968,21 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="45"/>
+      <c r="B17" s="69"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="45"/>
+      <c r="B18" s="69"/>
       <c r="C18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="84">
         <v>4.99</v>
       </c>
-      <c r="E18" s="60">
+      <c r="E18" s="84">
         <v>4.99</v>
       </c>
       <c r="F18" s="12" t="s">
@@ -2011,31 +2038,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="72" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="72" t="s">
+      <c r="E2" s="87"/>
+      <c r="F2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="72" t="s">
+      <c r="G2" s="87"/>
+      <c r="H2" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="73"/>
-      <c r="J2" s="72" t="s">
+      <c r="I2" s="87"/>
+      <c r="J2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="73"/>
+      <c r="K2" s="87"/>
       <c r="L2" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="5" t="s">
         <v>39</v>
       </c>
@@ -2065,30 +2092,30 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="88" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="77">
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="91">
         <v>2</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="77">
+      <c r="G4" s="92"/>
+      <c r="H4" s="91">
         <v>2</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="77">
+      <c r="I4" s="92"/>
+      <c r="J4" s="91">
         <v>1</v>
       </c>
-      <c r="K4" s="78"/>
+      <c r="K4" s="92"/>
       <c r="L4" s="24"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="75"/>
+      <c r="B5" s="89"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2124,7 +2151,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="75"/>
+      <c r="B6" s="89"/>
       <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
@@ -2160,7 +2187,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="75"/>
+      <c r="B7" s="89"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2196,20 +2223,20 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="75"/>
+      <c r="B8" s="89"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="42"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="66"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="75"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="3" t="s">
         <v>51</v>
       </c>
@@ -2244,7 +2271,7 @@
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="75"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="3" t="s">
         <v>52</v>
       </c>
@@ -2279,7 +2306,7 @@
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="75"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
@@ -2314,7 +2341,7 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="75"/>
+      <c r="B12" s="89"/>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
@@ -2349,20 +2376,20 @@
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="75"/>
+      <c r="B13" s="89"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="66"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="75"/>
+      <c r="B14" s="89"/>
       <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
@@ -2397,20 +2424,20 @@
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="75"/>
+      <c r="B15" s="89"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="76"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
@@ -2447,119 +2474,106 @@
       <c r="C18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="84">
         <f>SUM(E9:E12,E14,E16)</f>
         <v>50.74</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="62">
+      <c r="E18" s="67"/>
+      <c r="F18" s="93">
         <f>SUM(G5:G16)</f>
         <v>680.31</v>
       </c>
-      <c r="G18" s="63"/>
-      <c r="H18" s="62">
+      <c r="G18" s="94"/>
+      <c r="H18" s="93">
         <f>SUM(I5:I16)</f>
         <v>1789.18</v>
       </c>
-      <c r="I18" s="63"/>
-      <c r="J18" s="62">
+      <c r="I18" s="94"/>
+      <c r="J18" s="93">
         <f>SUM(K5:K16)</f>
         <v>3576.37</v>
       </c>
-      <c r="K18" s="63"/>
+      <c r="K18" s="94"/>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="67">
+      <c r="D19" s="98">
         <v>49.99</v>
       </c>
-      <c r="E19" s="68"/>
-      <c r="F19" s="62">
+      <c r="E19" s="99"/>
+      <c r="F19" s="93">
         <v>599.99</v>
       </c>
-      <c r="G19" s="63"/>
-      <c r="H19" s="62">
+      <c r="G19" s="94"/>
+      <c r="H19" s="93">
         <v>1499.99</v>
       </c>
-      <c r="I19" s="63"/>
-      <c r="J19" s="62">
+      <c r="I19" s="94"/>
+      <c r="J19" s="93">
         <v>2799.99</v>
       </c>
-      <c r="K19" s="63"/>
+      <c r="K19" s="94"/>
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="79">
+        <v>59</v>
+      </c>
+      <c r="D20" s="103">
         <f>(D19/D18)</f>
         <v>0.98521876231769812</v>
       </c>
-      <c r="E20" s="80"/>
-      <c r="F20" s="79">
+      <c r="E20" s="104"/>
+      <c r="F20" s="103">
         <f>(F19/F18)</f>
         <v>0.88193617615498821</v>
       </c>
-      <c r="G20" s="80"/>
-      <c r="H20" s="79">
+      <c r="G20" s="104"/>
+      <c r="H20" s="103">
         <f>(H19/H18)</f>
         <v>0.83836729675046662</v>
       </c>
-      <c r="I20" s="80"/>
-      <c r="J20" s="79">
+      <c r="I20" s="104"/>
+      <c r="J20" s="103">
         <f>(J19/J18)</f>
         <v>0.78291396024460558</v>
       </c>
-      <c r="K20" s="80"/>
+      <c r="K20" s="104"/>
       <c r="L20" s="8"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="69" t="s">
+      <c r="C22" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="71"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="101"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="101"/>
+      <c r="J22" s="101"/>
+      <c r="K22" s="101"/>
+      <c r="L22" s="102"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="66"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="D15:L15"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B4:B16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="C23:L23"/>
@@ -2574,6 +2588,19 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="D15:L15"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B4:B16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2582,10 +2609,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB03894-93D0-495C-B3BA-C4E55DD6402D}">
-  <dimension ref="B2:K22"/>
+  <dimension ref="B2:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,392 +2621,599 @@
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="81" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="105">
+      <c r="B2" s="113" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="40">
         <v>45017</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="86" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103"/>
+      <c r="B4" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="106">
+      <c r="E5" s="41">
         <v>7916.666666666667</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="94"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="106">
+      <c r="B6" s="106"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="41">
         <v>3333.3333333333298</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="94"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="85" t="s">
+      <c r="B7" s="106"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="106">
+      <c r="E7" s="41">
         <v>3750</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="94"/>
-      <c r="C8" s="99" t="s">
+      <c r="B8" s="106"/>
+      <c r="C8" s="108" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="100"/>
-      <c r="E8" s="106">
+      <c r="D8" s="109"/>
+      <c r="E8" s="41">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="94"/>
-      <c r="C9" s="99" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="100"/>
-      <c r="E9" s="106">
+      <c r="B9" s="106"/>
+      <c r="C9" s="108" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="109"/>
+      <c r="E9" s="41">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="95"/>
-      <c r="C10" s="99" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="100"/>
-      <c r="E10" s="106">
+      <c r="B10" s="107"/>
+      <c r="C10" s="108" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="109"/>
+      <c r="E10" s="41">
         <v>1671.9999999999998</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="96" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="107">
+      <c r="B11" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="42">
         <f>SUM(E5:E10)</f>
         <v>16871.999999999996</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="90" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="114" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="114"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="42">
+        <f>E11/9</f>
+        <v>1874.6666666666663</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="110" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="110"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="111"/>
+      <c r="D15" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="90"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91" t="s">
+      <c r="E15" s="111"/>
+      <c r="F15" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91" t="s">
+      <c r="G15" s="111"/>
+      <c r="H15" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="91"/>
-      <c r="J14" s="92" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="92" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="82">
+      <c r="I15" s="111"/>
+      <c r="J15" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="32">
         <v>338</v>
       </c>
-      <c r="C15" s="84">
+      <c r="C16" s="34">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D15" s="82">
+      <c r="D16" s="32">
         <v>0</v>
       </c>
-      <c r="E15" s="84">
+      <c r="E16" s="34">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F15" s="83">
+      <c r="F16" s="33">
         <v>0</v>
       </c>
-      <c r="G15" s="84">
+      <c r="G16" s="34">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H15" s="83">
+      <c r="H16" s="33">
         <v>0</v>
       </c>
-      <c r="I15" s="84">
+      <c r="I16" s="34">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J15" s="84">
-        <f>SUM((B15*C15),(D15*E15),(F15*G15),(H15*I15))</f>
+      <c r="J16" s="34">
+        <f>SUM((B16*C16),(D16*E16),(F16*G16),(H16*I16))</f>
         <v>16896.62</v>
       </c>
-      <c r="K15" s="97">
-        <f>SUM(B15,D15,F15,H15)</f>
+      <c r="K16" s="38">
+        <f>SUM(B16,D16,F16,H16)</f>
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="82">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="32">
         <v>0</v>
       </c>
-      <c r="C16" s="84">
+      <c r="C17" s="34">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D16" s="82">
+      <c r="D17" s="32">
         <v>29</v>
       </c>
-      <c r="E16" s="84">
+      <c r="E17" s="34">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F16" s="83">
+      <c r="F17" s="33">
         <v>0</v>
       </c>
-      <c r="G16" s="84">
+      <c r="G17" s="34">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H16" s="83">
+      <c r="H17" s="33">
         <v>0</v>
       </c>
-      <c r="I16" s="84">
+      <c r="I17" s="34">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J16" s="84">
-        <f>SUM((B16*C16),(D16*E16),(F16*G16),(H16*I16))</f>
+      <c r="J17" s="34">
+        <f>SUM((B17*C17),(D17*E17),(F17*G17),(H17*I17))</f>
         <v>17399.71</v>
       </c>
-      <c r="K16" s="97">
-        <f t="shared" ref="K16:K18" si="0">SUM(B16,D16,F16,H16)</f>
+      <c r="K17" s="38">
+        <f t="shared" ref="K17:K19" si="0">SUM(B17,D17,F17,H17)</f>
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="82">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="32">
         <v>0</v>
       </c>
-      <c r="C17" s="84">
+      <c r="C18" s="34">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D17" s="82">
+      <c r="D18" s="32">
         <v>0</v>
       </c>
-      <c r="E17" s="84">
+      <c r="E18" s="34">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F17" s="83">
+      <c r="F18" s="33">
         <v>12</v>
       </c>
-      <c r="G17" s="84">
+      <c r="G18" s="34">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H17" s="83">
+      <c r="H18" s="33">
         <v>0</v>
       </c>
-      <c r="I17" s="84">
+      <c r="I18" s="34">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J17" s="84">
-        <f>SUM((B17*C17),(D17*E17),(F17*G17),(H17*I17))</f>
+      <c r="J18" s="34">
+        <f>SUM((B18*C18),(D18*E18),(F18*G18),(H18*I18))</f>
         <v>17999.88</v>
       </c>
-      <c r="K17" s="97">
+      <c r="K18" s="38">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="82">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="32">
         <v>0</v>
       </c>
-      <c r="C18" s="84">
+      <c r="C19" s="34">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D18" s="82">
+      <c r="D19" s="32">
         <v>0</v>
       </c>
-      <c r="E18" s="84">
+      <c r="E19" s="34">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F18" s="83">
+      <c r="F19" s="33">
         <v>0</v>
       </c>
-      <c r="G18" s="84">
+      <c r="G19" s="34">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H18" s="83">
+      <c r="H19" s="33">
         <v>7</v>
       </c>
-      <c r="I18" s="84">
+      <c r="I19" s="34">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J18" s="84">
-        <f>SUM((B18*C18),(D18*E18),(F18*G18),(H18*I18))</f>
+      <c r="J19" s="34">
+        <f>SUM((B19*C19),(D19*E19),(F19*G19),(H19*I19))</f>
         <v>19599.93</v>
       </c>
-      <c r="K18" s="97">
+      <c r="K19" s="38">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="90" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="90"/>
-    </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="110" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="110"/>
+      <c r="G21" s="110"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="110"/>
+      <c r="K21" s="110"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91" t="s">
+      <c r="C22" s="111"/>
+      <c r="D22" s="111" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="91"/>
-      <c r="H21" s="91" t="s">
+      <c r="G22" s="111"/>
+      <c r="H22" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="91"/>
-      <c r="J21" s="92" t="s">
-        <v>64</v>
-      </c>
-      <c r="K21" s="92" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="82">
-        <v>0</v>
-      </c>
-      <c r="C22" s="84">
+      <c r="I22" s="111"/>
+      <c r="J22" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" s="37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="32">
+        <v>38</v>
+      </c>
+      <c r="C23" s="34">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D22" s="82">
+      <c r="D23" s="32">
         <v>0</v>
       </c>
-      <c r="E22" s="84">
+      <c r="E23" s="34">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F22" s="83">
+      <c r="F23" s="33">
         <v>0</v>
       </c>
-      <c r="G22" s="84">
+      <c r="G23" s="34">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H22" s="83">
+      <c r="H23" s="33">
         <v>0</v>
       </c>
-      <c r="I22" s="84">
+      <c r="I23" s="34">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J22" s="84">
-        <f>SUM((B22*C22),(D22*E22),(F22*G22),(H22*I22))</f>
+      <c r="J23" s="34">
+        <f>SUM((B23*C23),(D23*E23),(F23*G23),(H23*I23))</f>
+        <v>1899.6200000000001</v>
+      </c>
+      <c r="K23" s="38">
+        <f>SUM(B23,D23,F23,H23)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="32">
         <v>0</v>
       </c>
-      <c r="K22" s="97">
-        <f>SUM(B22,D22,F22,H22)</f>
+      <c r="C24" s="34">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D24" s="32">
+        <v>4</v>
+      </c>
+      <c r="E24" s="34">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F24" s="33">
         <v>0</v>
       </c>
+      <c r="G24" s="34">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+      <c r="I24" s="34">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J24" s="34">
+        <f>SUM((B24*C24),(D24*E24),(F24*G24),(H24*I24))</f>
+        <v>2399.96</v>
+      </c>
+      <c r="K24" s="38">
+        <f t="shared" ref="K24:K26" si="1">SUM(B24,D24,F24,H24)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="32">
+        <v>0</v>
+      </c>
+      <c r="C25" s="34">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D25" s="32">
+        <v>0</v>
+      </c>
+      <c r="E25" s="34">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F25" s="33">
+        <v>2</v>
+      </c>
+      <c r="G25" s="34">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H25" s="33">
+        <v>0</v>
+      </c>
+      <c r="I25" s="34">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J25" s="34">
+        <f>SUM((B25*C25),(D25*E25),(F25*G25),(H25*I25))</f>
+        <v>2999.98</v>
+      </c>
+      <c r="K25" s="38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="32">
+        <v>0</v>
+      </c>
+      <c r="C26" s="34">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D26" s="32">
+        <v>0</v>
+      </c>
+      <c r="E26" s="34">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0</v>
+      </c>
+      <c r="G26" s="34">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H26" s="33">
+        <v>1</v>
+      </c>
+      <c r="I26" s="34">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J26" s="34">
+        <f>SUM((B26*C26),(D26*E26),(F26*G26),(H26*I26))</f>
+        <v>2799.99</v>
+      </c>
+      <c r="K26" s="38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="125" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="126"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
+      <c r="H28" s="126"/>
+      <c r="I28" s="126"/>
+      <c r="J28" s="126"/>
+      <c r="K28" s="127"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="124"/>
+      <c r="D29" s="123" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="124"/>
+      <c r="F29" s="123" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="124"/>
+      <c r="H29" s="123" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="124"/>
+      <c r="J29" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" s="37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="32">
+        <v>100</v>
+      </c>
+      <c r="C30" s="34">
+        <f>'Package pricing'!$D$19</f>
+        <v>49.99</v>
+      </c>
+      <c r="D30" s="32">
+        <v>10</v>
+      </c>
+      <c r="E30" s="34">
+        <f>'Package pricing'!$F$19</f>
+        <v>599.99</v>
+      </c>
+      <c r="F30" s="33">
+        <v>5</v>
+      </c>
+      <c r="G30" s="34">
+        <f>'Package pricing'!$H$19</f>
+        <v>1499.99</v>
+      </c>
+      <c r="H30" s="33">
+        <v>1</v>
+      </c>
+      <c r="I30" s="34">
+        <f>'Package pricing'!$J$19</f>
+        <v>2799.99</v>
+      </c>
+      <c r="J30" s="34">
+        <f>SUM((B30*C30),(D30*E30),(F30*G30),(H30*I30))</f>
+        <v>21298.839999999997</v>
+      </c>
+      <c r="K30" s="38">
+        <f>SUM(B30,D30,F30,H30)</f>
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="23">
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B21:K21"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B14:K14"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2987,1138 +3221,1491 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F647B2FF-201C-44DE-9C82-A6B59556EC9F}">
-  <dimension ref="B2:P43"/>
+  <dimension ref="B2:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="108" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="43" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
     <col min="10" max="10" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="23.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="87" t="s">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="118" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="119"/>
+      <c r="D2" s="120"/>
+      <c r="F2" s="118" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="119"/>
+      <c r="H2" s="120"/>
+      <c r="J2" s="118" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="119"/>
+      <c r="L2" s="120"/>
+      <c r="N2" s="118" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" s="119"/>
+      <c r="P2" s="120"/>
+      <c r="R2" s="118" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="119"/>
+      <c r="T2" s="120"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="121" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="114"/>
+      <c r="F4" s="121" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="114"/>
+      <c r="J4" s="121" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="114"/>
+      <c r="N4" s="121" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" s="114"/>
+      <c r="R4" s="121" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="114"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="121"/>
+      <c r="C5" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="89"/>
-      <c r="F2" s="87" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" s="88"/>
-      <c r="H2" s="89"/>
-      <c r="J2" s="87" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="88"/>
-      <c r="L2" s="89"/>
-      <c r="N2" s="87" t="s">
-        <v>97</v>
-      </c>
-      <c r="O2" s="88"/>
-      <c r="P2" s="89"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="117" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="96"/>
-      <c r="F4" s="117" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="96"/>
-      <c r="J4" s="117" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="96"/>
-      <c r="N4" s="117" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" s="96"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="117"/>
-      <c r="C5" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="109">
+      <c r="D5" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F5" s="117"/>
-      <c r="G5" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="109">
+      <c r="F5" s="121"/>
+      <c r="G5" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J5" s="117"/>
-      <c r="K5" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="L5" s="109">
+      <c r="J5" s="121"/>
+      <c r="K5" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N5" s="117"/>
-      <c r="O5" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="P5" s="109">
+      <c r="N5" s="121"/>
+      <c r="O5" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="P5" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="117"/>
-      <c r="C6" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="109">
+      <c r="R5" s="121"/>
+      <c r="S5" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="T5" s="44">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="121"/>
+      <c r="C6" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="44">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="F6" s="117"/>
-      <c r="G6" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="109">
+      <c r="F6" s="121"/>
+      <c r="G6" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="44">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="J6" s="117"/>
-      <c r="K6" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" s="109">
+      <c r="J6" s="121"/>
+      <c r="K6" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="44">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="N6" s="117"/>
-      <c r="O6" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="P6" s="109">
+      <c r="N6" s="121"/>
+      <c r="O6" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" s="44">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="117"/>
-      <c r="C7" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="122" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="117"/>
-      <c r="G7" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="109">
+      <c r="R6" s="121"/>
+      <c r="S6" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="T6" s="44">
+        <f>40000/12</f>
+        <v>3333.3333333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="121"/>
+      <c r="C7" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="121"/>
+      <c r="G7" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="44">
         <f>12500+(H10*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="J7" s="117"/>
-      <c r="K7" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" s="109">
+      <c r="J7" s="121"/>
+      <c r="K7" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="44">
         <f>12500+(L10*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="N7" s="117"/>
-      <c r="O7" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="P7" s="109">
+      <c r="N7" s="121"/>
+      <c r="O7" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="P7" s="44">
         <f>12500+(P10*0.1)</f>
         <v>13062.4</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="117"/>
-      <c r="C8" s="96" t="s">
+      <c r="R7" s="121"/>
+      <c r="S7" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="96"/>
-      <c r="F8" s="117"/>
-      <c r="G8" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="96"/>
-      <c r="J8" s="117"/>
-      <c r="K8" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="L8" s="96"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="P8" s="96"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="117"/>
-      <c r="C9" s="119" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="120" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="117"/>
-      <c r="G9" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" s="109">
+      <c r="T7" s="44">
+        <f>12500+(T10*0.1)</f>
+        <v>13062.4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="121"/>
+      <c r="C8" s="114" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="114"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="114" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="114"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="114" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="114"/>
+      <c r="N8" s="121"/>
+      <c r="O8" s="114" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="114"/>
+      <c r="R8" s="121"/>
+      <c r="S8" s="114" t="s">
+        <v>77</v>
+      </c>
+      <c r="T8" s="114"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="121"/>
+      <c r="C9" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="121"/>
+      <c r="G9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="44">
         <f>SUM(D33+D34)</f>
         <v>16871.999999999996</v>
       </c>
-      <c r="J9" s="117"/>
-      <c r="K9" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="L9" s="109">
+      <c r="J9" s="121"/>
+      <c r="K9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="44">
         <f>SUM(H33+H34)</f>
         <v>39367.999999999993</v>
       </c>
-      <c r="N9" s="117"/>
-      <c r="O9" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="P9" s="109">
+      <c r="N9" s="121"/>
+      <c r="O9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" s="44">
         <f>SUM(L33+L34)</f>
         <v>61863.999999999993</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="117"/>
-      <c r="C10" s="121" t="s">
+      <c r="R9" s="121"/>
+      <c r="S9" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="T9" s="44">
+        <f>SUM(P33+P34)</f>
+        <v>84359.999999999985</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="121"/>
+      <c r="C10" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="121"/>
+      <c r="G10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="120" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="117"/>
-      <c r="G10" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="109">
+      <c r="H10" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J10" s="117"/>
-      <c r="K10" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="L10" s="109">
+      <c r="J10" s="121"/>
+      <c r="K10" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N10" s="117"/>
-      <c r="O10" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="P10" s="109">
+      <c r="N10" s="121"/>
+      <c r="O10" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="P10" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="113"/>
-      <c r="C11" s="114"/>
-      <c r="D11" s="115"/>
-      <c r="F11" s="113"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="115"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="114"/>
-      <c r="L11" s="115"/>
-      <c r="N11" s="113"/>
-      <c r="O11" s="114"/>
-      <c r="P11" s="115"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="96" t="s">
+      <c r="R10" s="121"/>
+      <c r="S10" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="T10" s="44">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="49"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="49"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="49"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="49"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="96"/>
-      <c r="F12" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="96" t="s">
+      <c r="D12" s="114"/>
+      <c r="F12" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="96"/>
-      <c r="J12" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="K12" s="96" t="s">
+      <c r="H12" s="114"/>
+      <c r="J12" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="K12" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="96"/>
-      <c r="N12" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="O12" s="96" t="s">
+      <c r="L12" s="114"/>
+      <c r="N12" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="O12" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="P12" s="96"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="94"/>
-      <c r="C13" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="109">
+      <c r="P12" s="114"/>
+      <c r="R12" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="S12" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="T12" s="114"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="106"/>
+      <c r="C13" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F13" s="94"/>
-      <c r="G13" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="109">
+      <c r="F13" s="106"/>
+      <c r="G13" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J13" s="94"/>
-      <c r="K13" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="L13" s="109">
+      <c r="J13" s="106"/>
+      <c r="K13" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N13" s="94"/>
-      <c r="O13" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="P13" s="109">
+      <c r="N13" s="106"/>
+      <c r="O13" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="P13" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="94"/>
-      <c r="C14" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="109">
+      <c r="R13" s="106"/>
+      <c r="S13" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="T13" s="44">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="106"/>
+      <c r="C14" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="44">
         <v>10000</v>
       </c>
-      <c r="F14" s="94"/>
-      <c r="G14" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="109">
+      <c r="F14" s="106"/>
+      <c r="G14" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="44">
         <v>10000</v>
       </c>
-      <c r="J14" s="94"/>
-      <c r="K14" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="L14" s="109">
+      <c r="J14" s="106"/>
+      <c r="K14" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="44">
         <v>10000</v>
       </c>
-      <c r="N14" s="94"/>
-      <c r="O14" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="P14" s="109">
+      <c r="N14" s="106"/>
+      <c r="O14" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" s="44">
         <v>10000</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="94"/>
-      <c r="C15" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="109">
+      <c r="R14" s="106"/>
+      <c r="S14" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="T14" s="44">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="106"/>
+      <c r="C15" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="44">
         <f>12500+(D18*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="F15" s="94"/>
-      <c r="G15" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="109">
+      <c r="F15" s="106"/>
+      <c r="G15" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="44">
         <f>12500+(H18*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="J15" s="94"/>
-      <c r="K15" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="L15" s="109">
+      <c r="J15" s="106"/>
+      <c r="K15" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="44">
         <f>12500+(L18*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="N15" s="94"/>
-      <c r="O15" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="P15" s="109">
+      <c r="N15" s="106"/>
+      <c r="O15" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="P15" s="44">
         <f>12500+(P18*0.1)</f>
         <v>13062.4</v>
       </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="94"/>
-      <c r="C16" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="96"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" s="96"/>
-      <c r="J16" s="94"/>
-      <c r="K16" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="L16" s="96"/>
-      <c r="N16" s="94"/>
-      <c r="O16" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="P16" s="96"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="94"/>
-      <c r="C17" s="119" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="120" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="94"/>
-      <c r="G17" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" s="123">
+      <c r="R15" s="106"/>
+      <c r="S15" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="T15" s="44">
+        <f>12500+(T18*0.1)</f>
+        <v>13062.4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="106"/>
+      <c r="C16" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="114"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="114"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="114"/>
+      <c r="N16" s="106"/>
+      <c r="O16" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="P16" s="114"/>
+      <c r="R16" s="106"/>
+      <c r="S16" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="T16" s="114"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="106"/>
+      <c r="C17" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="106"/>
+      <c r="G17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" s="54">
         <f>SUM(H9:H10)</f>
         <v>22495.999999999996</v>
       </c>
-      <c r="J17" s="94"/>
-      <c r="K17" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="123">
+      <c r="J17" s="106"/>
+      <c r="K17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" s="54">
         <f>SUM(L9:L10)</f>
         <v>44991.999999999993</v>
       </c>
-      <c r="N17" s="94"/>
-      <c r="O17" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="P17" s="123">
+      <c r="N17" s="106"/>
+      <c r="O17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="P17" s="54">
         <f>SUM(P9:P10)</f>
         <v>67487.999999999985</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="95"/>
-      <c r="C18" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="109">
+      <c r="R17" s="106"/>
+      <c r="S17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="T17" s="54">
+        <f>SUM(T9:T10)</f>
+        <v>89983.999999999985</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="107"/>
+      <c r="C18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F18" s="95"/>
-      <c r="G18" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="109">
+      <c r="F18" s="107"/>
+      <c r="G18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J18" s="95"/>
-      <c r="K18" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="L18" s="109">
+      <c r="J18" s="107"/>
+      <c r="K18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="L18" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N18" s="95"/>
-      <c r="O18" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="P18" s="109">
+      <c r="N18" s="107"/>
+      <c r="O18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="P18" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H19" s="108"/>
-      <c r="L19" s="108"/>
-      <c r="P19" s="108"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="118" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="96" t="s">
+      <c r="R18" s="107"/>
+      <c r="S18" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="T18" s="44">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="T19" s="43"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="96"/>
-      <c r="F20" s="118" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="96" t="s">
+      <c r="D20" s="114"/>
+      <c r="F20" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="96"/>
-      <c r="J20" s="118" t="s">
-        <v>85</v>
-      </c>
-      <c r="K20" s="96" t="s">
+      <c r="H20" s="114"/>
+      <c r="J20" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="L20" s="96"/>
-      <c r="N20" s="118" t="s">
-        <v>85</v>
-      </c>
-      <c r="O20" s="96" t="s">
+      <c r="L20" s="114"/>
+      <c r="N20" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="O20" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="P20" s="96"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="118"/>
-      <c r="C21" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="109">
+      <c r="P20" s="114"/>
+      <c r="R20" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="S20" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="T20" s="114"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="117"/>
+      <c r="C21" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F21" s="118"/>
-      <c r="G21" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="109">
+      <c r="F21" s="117"/>
+      <c r="G21" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J21" s="118"/>
-      <c r="K21" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="L21" s="109">
+      <c r="J21" s="117"/>
+      <c r="K21" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N21" s="118"/>
-      <c r="O21" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="P21" s="109">
+      <c r="N21" s="117"/>
+      <c r="O21" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="P21" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="118"/>
-      <c r="C22" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="109">
+      <c r="R21" s="117"/>
+      <c r="S21" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="T21" s="44">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="117"/>
+      <c r="C22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="44">
         <v>10000</v>
       </c>
-      <c r="F22" s="118"/>
-      <c r="G22" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="H22" s="109">
+      <c r="F22" s="117"/>
+      <c r="G22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="44">
         <v>10000</v>
       </c>
-      <c r="J22" s="118"/>
-      <c r="K22" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="L22" s="109">
+      <c r="J22" s="117"/>
+      <c r="K22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L22" s="44">
         <v>10000</v>
       </c>
-      <c r="N22" s="118"/>
-      <c r="O22" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="P22" s="109">
+      <c r="N22" s="117"/>
+      <c r="O22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="P22" s="44">
         <v>10000</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="118"/>
-      <c r="C23" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="109">
+      <c r="R22" s="117"/>
+      <c r="S22" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="T22" s="44">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="117"/>
+      <c r="C23" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="44">
         <f>12500+(D25*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="F23" s="118"/>
-      <c r="G23" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="H23" s="109">
+      <c r="F23" s="117"/>
+      <c r="G23" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="44">
         <f>12500+(H26*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="J23" s="118"/>
-      <c r="K23" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="L23" s="109">
+      <c r="J23" s="117"/>
+      <c r="K23" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="L23" s="44">
         <f>12500+(L26*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="N23" s="118"/>
-      <c r="O23" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="P23" s="109">
+      <c r="N23" s="117"/>
+      <c r="O23" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" s="44">
         <f>12500+(P26*0.1)</f>
         <v>13062.4</v>
       </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="118"/>
-      <c r="C24" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="96"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="96"/>
-      <c r="J24" s="118"/>
-      <c r="K24" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="L24" s="96"/>
-      <c r="N24" s="118"/>
-      <c r="O24" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="P24" s="96"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="118"/>
-      <c r="C25" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="109">
+      <c r="R23" s="117"/>
+      <c r="S23" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="T23" s="44">
+        <f>12500+(T26*0.1)</f>
+        <v>13062.4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="117"/>
+      <c r="C24" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="114"/>
+      <c r="F24" s="117"/>
+      <c r="G24" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="114"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="114"/>
+      <c r="N24" s="117"/>
+      <c r="O24" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="P24" s="114"/>
+      <c r="R24" s="117"/>
+      <c r="S24" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="T24" s="114"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="117"/>
+      <c r="C25" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="44">
         <f>D18</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F25" s="118"/>
-      <c r="G25" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="H25" s="109">
+      <c r="F25" s="117"/>
+      <c r="G25" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="44">
         <f>SUM(H17:H18)</f>
         <v>28119.999999999996</v>
       </c>
-      <c r="J25" s="118"/>
-      <c r="K25" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="L25" s="109">
+      <c r="J25" s="117"/>
+      <c r="K25" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L25" s="44">
         <f>SUM(L17:L18)</f>
         <v>50615.999999999993</v>
       </c>
-      <c r="N25" s="118"/>
-      <c r="O25" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="P25" s="109">
+      <c r="N25" s="117"/>
+      <c r="O25" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="P25" s="44">
         <f>SUM(P17:P18)</f>
         <v>73111.999999999985</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="118"/>
-      <c r="C26" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="109">
+      <c r="R25" s="117"/>
+      <c r="S25" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="T25" s="44">
+        <f>SUM(T17:T18)</f>
+        <v>95607.999999999985</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="117"/>
+      <c r="C26" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F26" s="118"/>
-      <c r="G26" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" s="109">
+      <c r="F26" s="117"/>
+      <c r="G26" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J26" s="118"/>
-      <c r="K26" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="L26" s="109">
+      <c r="J26" s="117"/>
+      <c r="K26" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N26" s="118"/>
-      <c r="O26" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="P26" s="109">
+      <c r="N26" s="117"/>
+      <c r="O26" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="P26" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H27" s="108"/>
-      <c r="L27" s="108"/>
-      <c r="P27" s="108"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="118" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="96" t="s">
+      <c r="R26" s="117"/>
+      <c r="S26" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="T26" s="44">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="T27" s="43"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="96"/>
-      <c r="F28" s="118" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="96" t="s">
+      <c r="D28" s="114"/>
+      <c r="F28" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="H28" s="96"/>
-      <c r="J28" s="118" t="s">
-        <v>88</v>
-      </c>
-      <c r="K28" s="96" t="s">
+      <c r="H28" s="114"/>
+      <c r="J28" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="K28" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="L28" s="96"/>
-      <c r="N28" s="118" t="s">
-        <v>88</v>
-      </c>
-      <c r="O28" s="96" t="s">
+      <c r="L28" s="114"/>
+      <c r="N28" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="O28" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="P28" s="96"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="118"/>
-      <c r="C29" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="109">
+      <c r="P28" s="114"/>
+      <c r="R28" s="117" t="s">
+        <v>85</v>
+      </c>
+      <c r="S28" s="114" t="s">
+        <v>53</v>
+      </c>
+      <c r="T28" s="114"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="117"/>
+      <c r="C29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F29" s="118"/>
-      <c r="G29" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="H29" s="109">
+      <c r="F29" s="117"/>
+      <c r="G29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J29" s="118"/>
-      <c r="K29" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="L29" s="109">
+      <c r="J29" s="117"/>
+      <c r="K29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L29" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N29" s="118"/>
-      <c r="O29" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="P29" s="109">
+      <c r="N29" s="117"/>
+      <c r="O29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="P29" s="44">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="118"/>
-      <c r="C30" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="109">
+      <c r="R29" s="117"/>
+      <c r="S29" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="T29" s="44">
+        <f>'Required sales'!$E$5*3</f>
+        <v>23750</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="117"/>
+      <c r="C30" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="44">
         <v>10000</v>
       </c>
-      <c r="F30" s="118"/>
-      <c r="G30" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="H30" s="109">
+      <c r="F30" s="117"/>
+      <c r="G30" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="44">
         <v>10000</v>
       </c>
-      <c r="J30" s="118"/>
-      <c r="K30" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="L30" s="109">
+      <c r="J30" s="117"/>
+      <c r="K30" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L30" s="44">
         <v>10000</v>
       </c>
-      <c r="N30" s="118"/>
-      <c r="O30" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="P30" s="109">
+      <c r="N30" s="117"/>
+      <c r="O30" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="P30" s="44">
         <v>10000</v>
       </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="118"/>
-      <c r="C31" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="109">
+      <c r="R30" s="117"/>
+      <c r="S30" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="T30" s="44">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="117"/>
+      <c r="C31" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="44">
         <f>12500+(D33*0.1)</f>
         <v>13624.8</v>
       </c>
-      <c r="F31" s="118"/>
-      <c r="G31" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="H31" s="109">
+      <c r="F31" s="117"/>
+      <c r="G31" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="44">
         <f>12500+(H33*0.1)</f>
         <v>15874.4</v>
       </c>
-      <c r="J31" s="118"/>
-      <c r="K31" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="L31" s="109">
+      <c r="J31" s="117"/>
+      <c r="K31" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="L31" s="44">
         <f>12500+(L33*0.1)</f>
         <v>18124</v>
       </c>
-      <c r="N31" s="118"/>
-      <c r="O31" s="111" t="s">
-        <v>83</v>
-      </c>
-      <c r="P31" s="109">
+      <c r="N31" s="117"/>
+      <c r="O31" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="P31" s="44">
         <f>12500+(P33*0.1)</f>
         <v>20373.599999999999</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="118"/>
-      <c r="C32" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="96"/>
-      <c r="F32" s="118"/>
-      <c r="G32" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="96"/>
-      <c r="J32" s="118"/>
-      <c r="K32" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="L32" s="96"/>
-      <c r="N32" s="118"/>
-      <c r="O32" s="96" t="s">
-        <v>82</v>
-      </c>
-      <c r="P32" s="96"/>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="118"/>
-      <c r="C33" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="109">
+      <c r="R31" s="117"/>
+      <c r="S31" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="T31" s="44">
+        <f>12500+(T33*0.1)</f>
+        <v>22623.199999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="117"/>
+      <c r="C32" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="114"/>
+      <c r="F32" s="117"/>
+      <c r="G32" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="114"/>
+      <c r="J32" s="117"/>
+      <c r="K32" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="L32" s="114"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="P32" s="114"/>
+      <c r="R32" s="117"/>
+      <c r="S32" s="114" t="s">
+        <v>79</v>
+      </c>
+      <c r="T32" s="114"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="117"/>
+      <c r="C33" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="44">
         <f>D25+D26</f>
         <v>11247.999999999998</v>
       </c>
-      <c r="F33" s="118"/>
-      <c r="G33" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="H33" s="109">
+      <c r="F33" s="117"/>
+      <c r="G33" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="44">
         <f>H25+H26</f>
         <v>33743.999999999993</v>
       </c>
-      <c r="J33" s="118"/>
-      <c r="K33" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="L33" s="109">
+      <c r="J33" s="117"/>
+      <c r="K33" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="L33" s="44">
         <f>L25+L26</f>
         <v>56239.999999999993</v>
       </c>
-      <c r="N33" s="118"/>
-      <c r="O33" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="P33" s="109">
+      <c r="N33" s="117"/>
+      <c r="O33" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="P33" s="44">
         <f>P25+P26</f>
         <v>78735.999999999985</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="118"/>
-      <c r="C34" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="109">
+      <c r="R33" s="117"/>
+      <c r="S33" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="T33" s="44">
+        <f>T25+T26</f>
+        <v>101231.99999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="117"/>
+      <c r="C34" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F34" s="118"/>
-      <c r="G34" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="109">
+      <c r="F34" s="117"/>
+      <c r="G34" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J34" s="118"/>
-      <c r="K34" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="L34" s="109">
+      <c r="J34" s="117"/>
+      <c r="K34" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="L34" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N34" s="118"/>
-      <c r="O34" s="82" t="s">
-        <v>87</v>
-      </c>
-      <c r="P34" s="109">
+      <c r="N34" s="117"/>
+      <c r="O34" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="P34" s="44">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H35" s="108"/>
-      <c r="L35" s="108"/>
-      <c r="P35" s="108"/>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="110" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="110"/>
-      <c r="D36" s="109">
+      <c r="R34" s="117"/>
+      <c r="S34" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="T34" s="44">
+        <f>'Required sales'!$E$11/3</f>
+        <v>5623.9999999999991</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="P35" s="43"/>
+      <c r="T35" s="43"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="115"/>
+      <c r="D36" s="44">
         <f>SUM(D18,D25:D26,D33:D34)</f>
         <v>33743.999999999993</v>
       </c>
-      <c r="F36" s="110" t="s">
-        <v>90</v>
-      </c>
-      <c r="G36" s="110"/>
-      <c r="H36" s="109">
+      <c r="F36" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="115"/>
+      <c r="H36" s="44">
         <f>SUM(H9:H10,H17:H18,H25:H26,H33:H34)</f>
         <v>123727.99999999997</v>
       </c>
-      <c r="J36" s="110" t="s">
-        <v>90</v>
-      </c>
-      <c r="K36" s="110"/>
-      <c r="L36" s="109">
+      <c r="J36" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="K36" s="115"/>
+      <c r="L36" s="44">
         <f>SUM(L9:L10,L17:L18,L25:L26,L33:L34)</f>
         <v>213711.99999999997</v>
       </c>
-      <c r="N36" s="110" t="s">
-        <v>90</v>
-      </c>
-      <c r="O36" s="110"/>
-      <c r="P36" s="109">
+      <c r="N36" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="O36" s="115"/>
+      <c r="P36" s="44">
         <f>SUM(P9:P10,P17:P18,P25:P26,P33:P34)</f>
         <v>303695.99999999994</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="110"/>
-      <c r="D37" s="109">
+      <c r="R36" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="S36" s="115"/>
+      <c r="T36" s="44">
+        <f>SUM(T9:T10,T17:T18,T25:T26,T33:T34)</f>
+        <v>393679.99999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="115"/>
+      <c r="D37" s="44">
         <f>SUM(D5:D6,D13:D15,D21:D23,D29:D31)</f>
         <v>168082.93333333329</v>
       </c>
-      <c r="F37" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="G37" s="110"/>
-      <c r="H37" s="109">
+      <c r="F37" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="115"/>
+      <c r="H37" s="44">
         <f>SUM(H5:H6,H13:H15,H21:H23,H29:H31)</f>
         <v>170332.5333333333</v>
       </c>
-      <c r="J37" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="K37" s="110"/>
-      <c r="L37" s="109">
+      <c r="J37" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="K37" s="115"/>
+      <c r="L37" s="44">
         <f>SUM(L5:L6,L13:L15,L21:L23,L29:L31)</f>
         <v>172582.1333333333</v>
       </c>
-      <c r="N37" s="110" t="s">
-        <v>91</v>
-      </c>
-      <c r="O37" s="110"/>
-      <c r="P37" s="109">
+      <c r="N37" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="O37" s="115"/>
+      <c r="P37" s="44">
         <f>SUM(P5:P6,P13:P15,P21:P23,P29:P31)</f>
         <v>174831.73333333331</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H38" s="108"/>
-      <c r="L38" s="108"/>
-      <c r="P38" s="108"/>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="98"/>
-      <c r="D39" s="109">
-        <f>0-(D37-D36)</f>
+      <c r="R37" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="S37" s="115"/>
+      <c r="T37" s="44">
+        <f>SUM(T5:T6,T13:T15,T21:T23,T29:T31)</f>
+        <v>177081.33333333331</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="T38" s="43"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="116" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="116"/>
+      <c r="D39" s="44">
+        <f>0-D37+D36</f>
         <v>-134338.93333333329</v>
       </c>
-      <c r="F39" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="98"/>
-      <c r="H39" s="109">
-        <f>0-(H37-H36)</f>
+      <c r="F39" s="116" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" s="116"/>
+      <c r="H39" s="44">
+        <f>0-H37+H36</f>
         <v>-46604.533333333326</v>
       </c>
-      <c r="J39" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="K39" s="98"/>
-      <c r="L39" s="109">
-        <f>L37-L36</f>
-        <v>-41129.866666666669</v>
-      </c>
-      <c r="N39" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="O39" s="98"/>
-      <c r="P39" s="109">
-        <f>P37-P36</f>
-        <v>-128864.26666666663</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="98"/>
-      <c r="D40" s="109">
+      <c r="J39" s="116" t="s">
+        <v>90</v>
+      </c>
+      <c r="K39" s="116"/>
+      <c r="L39" s="44">
+        <f>0-L37+L36</f>
+        <v>41129.866666666669</v>
+      </c>
+      <c r="N39" s="116" t="s">
+        <v>90</v>
+      </c>
+      <c r="O39" s="116"/>
+      <c r="P39" s="44">
+        <f>0-P37+P36</f>
+        <v>128864.26666666663</v>
+      </c>
+      <c r="R39" s="116" t="s">
+        <v>90</v>
+      </c>
+      <c r="S39" s="116"/>
+      <c r="T39" s="44">
+        <f>0-T37+T36</f>
+        <v>216598.66666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="116"/>
+      <c r="D40" s="44">
         <f>D39</f>
         <v>-134338.93333333329</v>
       </c>
-      <c r="F40" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="G40" s="98"/>
-      <c r="H40" s="109">
-        <f>0-(D40+H39)</f>
-        <v>180943.46666666662</v>
-      </c>
-      <c r="J40" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="K40" s="98"/>
-      <c r="L40" s="109">
+      <c r="F40" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="116"/>
+      <c r="H40" s="44">
+        <f>D40+H39</f>
+        <v>-180943.46666666662</v>
+      </c>
+      <c r="J40" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="K40" s="116"/>
+      <c r="L40" s="44">
         <f>H40+L39</f>
-        <v>139813.59999999995</v>
-      </c>
-      <c r="N40" s="98" t="s">
-        <v>94</v>
-      </c>
-      <c r="O40" s="98"/>
-      <c r="P40" s="109">
+        <v>-139813.59999999995</v>
+      </c>
+      <c r="N40" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="O40" s="116"/>
+      <c r="P40" s="44">
         <f>L40+P39</f>
-        <v>10949.333333333314</v>
-      </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="98" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="98"/>
-      <c r="D42" s="98"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="98"/>
-      <c r="G42" s="98"/>
-      <c r="H42" s="98"/>
-      <c r="I42" s="98"/>
-      <c r="J42" s="98"/>
-      <c r="K42" s="98"/>
-    </row>
-    <row r="43" spans="2:16" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="116" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="102"/>
-      <c r="D43" s="102"/>
-      <c r="E43" s="102"/>
-      <c r="F43" s="102"/>
-      <c r="G43" s="102"/>
-      <c r="H43" s="102"/>
-      <c r="I43" s="102"/>
-      <c r="J43" s="102"/>
-      <c r="K43" s="102"/>
+        <v>-10949.333333333314</v>
+      </c>
+      <c r="R40" s="116" t="s">
+        <v>91</v>
+      </c>
+      <c r="S40" s="116"/>
+      <c r="T40" s="44">
+        <f>P40+T39</f>
+        <v>205649.33333333331</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="116" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="116"/>
+      <c r="D42" s="116"/>
+      <c r="E42" s="116"/>
+      <c r="F42" s="116"/>
+      <c r="G42" s="116"/>
+      <c r="H42" s="116"/>
+      <c r="I42" s="116"/>
+      <c r="J42" s="116"/>
+      <c r="K42" s="116"/>
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+      <c r="N42" s="116"/>
+      <c r="O42" s="116"/>
+      <c r="P42" s="116"/>
+      <c r="Q42" s="116"/>
+      <c r="R42" s="116"/>
+      <c r="S42" s="116"/>
+      <c r="T42" s="116"/>
+    </row>
+    <row r="43" spans="2:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="122" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="122"/>
+      <c r="D43" s="122"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="122"/>
+      <c r="G43" s="122"/>
+      <c r="H43" s="122"/>
+      <c r="I43" s="122"/>
+      <c r="J43" s="122"/>
+      <c r="K43" s="122"/>
+      <c r="L43" s="122"/>
+      <c r="M43" s="122"/>
+      <c r="N43" s="122"/>
+      <c r="O43" s="122"/>
+      <c r="P43" s="122"/>
+      <c r="Q43" s="122"/>
+      <c r="R43" s="122"/>
+      <c r="S43" s="122"/>
+      <c r="T43" s="122"/>
     </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="87">
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="B42:T42"/>
+    <mergeCell ref="R20:R26"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="R28:R34"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R4:R10"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="R12:R18"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B43:T43"/>
+    <mergeCell ref="F12:F18"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F20:F26"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="F28:F34"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="F4:F10"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="J28:J34"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="J20:J26"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="J12:J18"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N4:N10"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="N12:N18"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
     <mergeCell ref="N36:O36"/>
     <mergeCell ref="N37:O37"/>
     <mergeCell ref="N39:O39"/>
@@ -4129,88 +4716,28 @@
     <mergeCell ref="N28:N34"/>
     <mergeCell ref="O28:P28"/>
     <mergeCell ref="O32:P32"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N4:N10"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="N12:N18"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="J20:J26"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="J28:J34"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="F4:F10"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="J12:J18"/>
-    <mergeCell ref="F20:F26"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="F28:F34"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="F12:F18"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="D39:D40">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L39:L40 H39:H40">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="H39:H40 L39:L40 P39:P40">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P39:P40">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="T39:T40">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Version 1.1.3.1: More selector fixes. Logging page fixes.
</commit_message>
<xml_diff>
--- a/documents/Features.xlsx
+++ b/documents/Features.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Node\Timelog\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bundion Timelog\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872C793D-8BEC-496E-AC08-41401240F406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AA2E44-8B8D-41C9-807F-BE64DFD5D8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{DC53B2B3-FCDA-4DCD-BBF4-AC4638DF1791}"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="1" r:id="rId1"/>
     <sheet name="Prices" sheetId="2" r:id="rId2"/>
     <sheet name="Package pricing" sheetId="3" r:id="rId3"/>
     <sheet name="Required sales" sheetId="4" r:id="rId4"/>
-    <sheet name="2003 Projections" sheetId="5" r:id="rId5"/>
+    <sheet name="2023 Projections" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -675,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -683,11 +683,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -738,19 +738,16 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -760,29 +757,27 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -884,6 +879,42 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,47 +930,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -956,21 +963,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -994,27 +1004,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="6">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1035,50 +1030,6 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FF008000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
@@ -1415,7 +1366,7 @@
   <dimension ref="B2:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,32 +1380,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="68" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1426,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="66" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1501,7 +1452,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1476,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="69"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1549,17 +1500,17 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="69"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="66"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="69"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
@@ -1581,7 +1532,7 @@
       <c r="I10" s="8"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="69"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1594,14 +1545,14 @@
       <c r="F11" s="7">
         <v>20</v>
       </c>
-      <c r="G11" s="67" t="s">
+      <c r="G11" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="67"/>
+      <c r="H11" s="64"/>
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1614,14 +1565,14 @@
       <c r="F12" s="9">
         <v>100</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="67"/>
+      <c r="H12" s="64"/>
       <c r="I12" s="8"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1631,61 +1582,61 @@
       <c r="E13" s="7">
         <v>50</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="56"/>
-      <c r="H13" s="57"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="54"/>
       <c r="I13" s="8"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="69"/>
-      <c r="C14" s="28" t="s">
+      <c r="B14" s="66"/>
+      <c r="C14" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="71" t="s">
+      <c r="E14" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="29"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
-      <c r="C15" s="28" t="s">
+      <c r="B15" s="66"/>
+      <c r="C15" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="73"/>
-      <c r="F15" s="30">
+      <c r="E15" s="70"/>
+      <c r="F15" s="29">
         <v>5</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="29">
         <v>25</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="28"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="69"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="66"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="63"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="69"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1695,57 +1646,57 @@
       <c r="E17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="57"/>
+      <c r="G17" s="54"/>
       <c r="H17" s="7" t="s">
         <v>28</v>
       </c>
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="69"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="57"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="69"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="7">
         <v>1</v>
       </c>
-      <c r="F19" s="55">
+      <c r="F19" s="52">
         <v>5</v>
       </c>
-      <c r="G19" s="57">
+      <c r="G19" s="54">
         <v>25</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I19" s="8"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="60"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1775,7 +1726,7 @@
   <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:F12"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,17 +1740,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="74" t="s">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="76"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="73"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
       <c r="D3" s="18" t="s">
         <v>23</v>
       </c>
@@ -1811,111 +1762,111 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="66" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="84">
+      <c r="D4" s="81">
         <v>9.99</v>
       </c>
-      <c r="E4" s="84"/>
+      <c r="E4" s="81"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="84">
+      <c r="D5" s="81">
         <v>5.99</v>
       </c>
-      <c r="E5" s="84"/>
+      <c r="E5" s="81"/>
       <c r="F5" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="84">
+      <c r="D6" s="81">
         <v>2.99</v>
       </c>
-      <c r="E6" s="84"/>
+      <c r="E6" s="81"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="57"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="54"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="69"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="84">
+      <c r="D8" s="81">
         <v>0.99</v>
       </c>
-      <c r="E8" s="84"/>
+      <c r="E8" s="81"/>
       <c r="F8" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="69"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="84">
+      <c r="D9" s="81">
         <v>0.99</v>
       </c>
-      <c r="E9" s="84"/>
+      <c r="E9" s="81"/>
       <c r="F9" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="69"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="84">
+      <c r="D10" s="81">
         <v>0.49</v>
       </c>
-      <c r="E10" s="84"/>
+      <c r="E10" s="81"/>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="69"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="84">
+      <c r="D11" s="81">
         <v>0.12</v>
       </c>
-      <c r="E11" s="84"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="69"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
-      <c r="C13" s="77" t="s">
+      <c r="B13" s="66"/>
+      <c r="C13" s="74" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1929,8 +1880,8 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="69"/>
-      <c r="C14" s="78"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="7" t="s">
         <v>24</v>
       </c>
@@ -1942,8 +1893,8 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="69"/>
-      <c r="C15" s="78"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="7" t="s">
         <v>25</v>
       </c>
@@ -1955,8 +1906,8 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="69"/>
-      <c r="C16" s="79"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="76"/>
       <c r="D16" s="7" t="s">
         <v>28</v>
       </c>
@@ -1968,21 +1919,21 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="69"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="57"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="54"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="69"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="84">
+      <c r="D18" s="81">
         <v>4.99</v>
       </c>
-      <c r="E18" s="84">
+      <c r="E18" s="81">
         <v>4.99</v>
       </c>
       <c r="F18" s="12" t="s">
@@ -2038,31 +1989,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="86" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="86" t="s">
+      <c r="E2" s="96"/>
+      <c r="F2" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="86" t="s">
+      <c r="G2" s="96"/>
+      <c r="H2" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="87"/>
-      <c r="J2" s="86" t="s">
+      <c r="I2" s="96"/>
+      <c r="J2" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="87"/>
+      <c r="K2" s="96"/>
       <c r="L2" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="5" t="s">
         <v>39</v>
       </c>
@@ -2092,30 +2043,30 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="97" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="91"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="91">
+      <c r="D4" s="100"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="100">
         <v>2</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="91">
+      <c r="G4" s="101"/>
+      <c r="H4" s="100">
         <v>2</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="91">
+      <c r="I4" s="101"/>
+      <c r="J4" s="100">
         <v>1</v>
       </c>
-      <c r="K4" s="92"/>
+      <c r="K4" s="101"/>
       <c r="L4" s="24"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="89"/>
+      <c r="B5" s="98"/>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2151,7 +2102,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="89"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
@@ -2187,7 +2138,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="89"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2223,20 +2174,20 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="89"/>
+      <c r="B8" s="98"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="66"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="89"/>
+      <c r="B9" s="98"/>
       <c r="C9" s="3" t="s">
         <v>51</v>
       </c>
@@ -2271,7 +2222,7 @@
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="89"/>
+      <c r="B10" s="98"/>
       <c r="C10" s="3" t="s">
         <v>52</v>
       </c>
@@ -2306,7 +2257,7 @@
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="89"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
@@ -2341,7 +2292,7 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="89"/>
+      <c r="B12" s="98"/>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
@@ -2376,20 +2327,20 @@
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="89"/>
+      <c r="B13" s="98"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="66"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="63"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="89"/>
+      <c r="B14" s="98"/>
       <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
@@ -2424,24 +2375,24 @@
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="89"/>
+      <c r="B15" s="98"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="57"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="54"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="90"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="7">
         <v>1</v>
       </c>
       <c r="E16" s="21">
@@ -2474,106 +2425,119 @@
       <c r="C18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="84">
+      <c r="D18" s="81">
         <f>SUM(E9:E12,E14,E16)</f>
         <v>50.74</v>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="93">
+      <c r="E18" s="64"/>
+      <c r="F18" s="83">
         <f>SUM(G5:G16)</f>
         <v>680.31</v>
       </c>
-      <c r="G18" s="94"/>
-      <c r="H18" s="93">
+      <c r="G18" s="84"/>
+      <c r="H18" s="83">
         <f>SUM(I5:I16)</f>
         <v>1789.18</v>
       </c>
-      <c r="I18" s="94"/>
-      <c r="J18" s="93">
+      <c r="I18" s="84"/>
+      <c r="J18" s="83">
         <f>SUM(K5:K16)</f>
         <v>3576.37</v>
       </c>
-      <c r="K18" s="94"/>
+      <c r="K18" s="84"/>
       <c r="L18" s="8"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="98">
+      <c r="D19" s="88">
         <v>49.99</v>
       </c>
-      <c r="E19" s="99"/>
-      <c r="F19" s="93">
+      <c r="E19" s="89"/>
+      <c r="F19" s="83">
         <v>599.99</v>
       </c>
-      <c r="G19" s="94"/>
-      <c r="H19" s="93">
+      <c r="G19" s="84"/>
+      <c r="H19" s="83">
         <v>1499.99</v>
       </c>
-      <c r="I19" s="94"/>
-      <c r="J19" s="93">
+      <c r="I19" s="84"/>
+      <c r="J19" s="83">
         <v>2799.99</v>
       </c>
-      <c r="K19" s="94"/>
+      <c r="K19" s="84"/>
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="103">
+      <c r="D20" s="93">
         <f>(D19/D18)</f>
         <v>0.98521876231769812</v>
       </c>
-      <c r="E20" s="104"/>
-      <c r="F20" s="103">
+      <c r="E20" s="94"/>
+      <c r="F20" s="93">
         <f>(F19/F18)</f>
         <v>0.88193617615498821</v>
       </c>
-      <c r="G20" s="104"/>
-      <c r="H20" s="103">
+      <c r="G20" s="94"/>
+      <c r="H20" s="93">
         <f>(H19/H18)</f>
         <v>0.83836729675046662</v>
       </c>
-      <c r="I20" s="104"/>
-      <c r="J20" s="103">
+      <c r="I20" s="94"/>
+      <c r="J20" s="93">
         <f>(J19/J18)</f>
         <v>0.78291396024460558</v>
       </c>
-      <c r="K20" s="104"/>
+      <c r="K20" s="94"/>
       <c r="L20" s="8"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="101"/>
-      <c r="I22" s="101"/>
-      <c r="J22" s="101"/>
-      <c r="K22" s="101"/>
-      <c r="L22" s="102"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
+      <c r="F22" s="91"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
+      <c r="J22" s="91"/>
+      <c r="K22" s="91"/>
+      <c r="L22" s="92"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="97"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="D15:L15"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B4:B16"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="C23:L23"/>
@@ -2588,19 +2552,6 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="D15:L15"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B4:B16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2611,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB03894-93D0-495C-B3BA-C4E55DD6402D}">
   <dimension ref="B2:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,576 +2572,583 @@
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="30" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="40">
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="39">
         <v>45017</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="40">
         <v>7916.666666666667</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="106"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="35" t="s">
+      <c r="B6" s="107"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="40">
         <v>3333.3333333333298</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="106"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="35" t="s">
+      <c r="B7" s="107"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="40">
         <v>3750</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="106"/>
-      <c r="C8" s="108" t="s">
+      <c r="B8" s="107"/>
+      <c r="C8" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="109"/>
-      <c r="E8" s="41">
+      <c r="D8" s="110"/>
+      <c r="E8" s="40">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="106"/>
-      <c r="C9" s="108" t="s">
+      <c r="B9" s="107"/>
+      <c r="C9" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="109"/>
-      <c r="E9" s="41">
+      <c r="D9" s="110"/>
+      <c r="E9" s="40">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="107"/>
-      <c r="C10" s="108" t="s">
+      <c r="B10" s="108"/>
+      <c r="C10" s="109" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="41">
+      <c r="D10" s="110"/>
+      <c r="E10" s="40">
         <v>1671.9999999999998</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="103" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="114"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="42">
+      <c r="C11" s="103"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="41">
         <f>SUM(E5:E10)</f>
         <v>16871.999999999996</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="103" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="42">
+      <c r="C12" s="103"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="41">
         <f>E11/9</f>
         <v>1874.6666666666663</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="111" t="s">
+      <c r="B15" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111" t="s">
+      <c r="C15" s="102"/>
+      <c r="D15" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111" t="s">
+      <c r="E15" s="102"/>
+      <c r="F15" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111" t="s">
+      <c r="G15" s="102"/>
+      <c r="H15" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="111"/>
-      <c r="J15" s="37" t="s">
+      <c r="I15" s="102"/>
+      <c r="J15" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="36" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="32">
+      <c r="B16" s="31">
         <v>338</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>0</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="32">
         <v>0</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G16" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H16" s="33">
+      <c r="H16" s="32">
         <v>0</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="33">
         <f>SUM((B16*C16),(D16*E16),(F16*G16),(H16*I16))</f>
         <v>16896.62</v>
       </c>
-      <c r="K16" s="38">
+      <c r="K16" s="37">
         <f>SUM(B16,D16,F16,H16)</f>
         <v>338</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="32">
+      <c r="B17" s="31">
         <v>0</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>29</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <v>0</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="32">
         <v>0</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="33">
         <f>SUM((B17*C17),(D17*E17),(F17*G17),(H17*I17))</f>
         <v>17399.71</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="37">
         <f t="shared" ref="K17:K19" si="0">SUM(B17,D17,F17,H17)</f>
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="32">
+      <c r="B18" s="31">
         <v>0</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <v>0</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="32">
         <v>12</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="32">
         <v>0</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="33">
         <f>SUM((B18*C18),(D18*E18),(F18*G18),(H18*I18))</f>
         <v>17999.88</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K18" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="32">
+      <c r="B19" s="31">
         <v>0</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="31">
         <v>0</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="32">
         <v>0</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H19" s="33">
+      <c r="H19" s="32">
         <v>7</v>
       </c>
-      <c r="I19" s="34">
+      <c r="I19" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="33">
         <f>SUM((B19*C19),(D19*E19),(F19*G19),(H19*I19))</f>
         <v>19599.93</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K19" s="37">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="110" t="s">
+      <c r="B21" s="105" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="110"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="105"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="105"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="111"/>
-      <c r="D22" s="111" t="s">
+      <c r="C22" s="102"/>
+      <c r="D22" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="111"/>
-      <c r="F22" s="111" t="s">
+      <c r="E22" s="102"/>
+      <c r="F22" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="111"/>
-      <c r="H22" s="111" t="s">
+      <c r="G22" s="102"/>
+      <c r="H22" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="111"/>
-      <c r="J22" s="37" t="s">
+      <c r="I22" s="102"/>
+      <c r="J22" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="37" t="s">
+      <c r="K22" s="36" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32">
+      <c r="B23" s="31">
         <v>38</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <v>0</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="32">
         <v>0</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H23" s="33">
+      <c r="H23" s="32">
         <v>0</v>
       </c>
-      <c r="I23" s="34">
+      <c r="I23" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J23" s="34">
+      <c r="J23" s="33">
         <f>SUM((B23*C23),(D23*E23),(F23*G23),(H23*I23))</f>
         <v>1899.6200000000001</v>
       </c>
-      <c r="K23" s="38">
+      <c r="K23" s="37">
         <f>SUM(B23,D23,F23,H23)</f>
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="32">
+      <c r="B24" s="31">
         <v>0</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>4</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="32">
         <v>0</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H24" s="33">
+      <c r="H24" s="32">
         <v>0</v>
       </c>
-      <c r="I24" s="34">
+      <c r="I24" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="33">
         <f>SUM((B24*C24),(D24*E24),(F24*G24),(H24*I24))</f>
         <v>2399.96</v>
       </c>
-      <c r="K24" s="38">
+      <c r="K24" s="37">
         <f t="shared" ref="K24:K26" si="1">SUM(B24,D24,F24,H24)</f>
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="32">
+      <c r="B25" s="31">
         <v>0</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <v>0</v>
       </c>
-      <c r="E25" s="34">
+      <c r="E25" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="32">
         <v>2</v>
       </c>
-      <c r="G25" s="34">
+      <c r="G25" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H25" s="33">
+      <c r="H25" s="32">
         <v>0</v>
       </c>
-      <c r="I25" s="34">
+      <c r="I25" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J25" s="34">
+      <c r="J25" s="33">
         <f>SUM((B25*C25),(D25*E25),(F25*G25),(H25*I25))</f>
         <v>2999.98</v>
       </c>
-      <c r="K25" s="38">
+      <c r="K25" s="37">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <v>0</v>
       </c>
-      <c r="C26" s="34">
+      <c r="C26" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>0</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="32">
         <v>0</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H26" s="33">
+      <c r="H26" s="32">
         <v>1</v>
       </c>
-      <c r="I26" s="34">
+      <c r="I26" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J26" s="34">
+      <c r="J26" s="33">
         <f>SUM((B26*C26),(D26*E26),(F26*G26),(H26*I26))</f>
         <v>2799.99</v>
       </c>
-      <c r="K26" s="38">
+      <c r="K26" s="37">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="125" t="s">
+      <c r="B28" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="126"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="126"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="126"/>
-      <c r="I28" s="126"/>
-      <c r="J28" s="126"/>
-      <c r="K28" s="127"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="112"/>
+      <c r="G28" s="112"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="112"/>
+      <c r="J28" s="112"/>
+      <c r="K28" s="113"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="123" t="s">
+      <c r="B29" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="124"/>
-      <c r="D29" s="123" t="s">
+      <c r="C29" s="115"/>
+      <c r="D29" s="114" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="124"/>
-      <c r="F29" s="123" t="s">
+      <c r="E29" s="115"/>
+      <c r="F29" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="124"/>
-      <c r="H29" s="123" t="s">
+      <c r="G29" s="115"/>
+      <c r="H29" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="124"/>
-      <c r="J29" s="37" t="s">
+      <c r="I29" s="115"/>
+      <c r="J29" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="K29" s="37" t="s">
+      <c r="K29" s="36" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="32">
+      <c r="B30" s="31">
         <v>100</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="33">
         <f>'Package pricing'!$D$19</f>
         <v>49.99</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="31">
         <v>10</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E30" s="33">
         <f>'Package pricing'!$F$19</f>
         <v>599.99</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="32">
         <v>5</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="33">
         <f>'Package pricing'!$H$19</f>
         <v>1499.99</v>
       </c>
-      <c r="H30" s="33">
+      <c r="H30" s="32">
         <v>1</v>
       </c>
-      <c r="I30" s="34">
+      <c r="I30" s="33">
         <f>'Package pricing'!$J$19</f>
         <v>2799.99</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="33">
         <f>SUM((B30*C30),(D30*E30),(F30*G30),(H30*I30))</f>
         <v>21298.839999999997</v>
       </c>
-      <c r="K30" s="38">
+      <c r="K30" s="37">
         <f>SUM(B30,D30,F30,H30)</f>
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:D2"/>
@@ -3200,11 +3158,6 @@
     <mergeCell ref="B21:K21"/>
     <mergeCell ref="B5:B10"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="B14:K14"/>
@@ -3212,8 +3165,6 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3223,8 +3174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F647B2FF-201C-44DE-9C82-A6B59556EC9F}">
   <dimension ref="B2:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,7 +3183,7 @@
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="43" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="42" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" customWidth="1"/>
@@ -3252,1407 +3203,1419 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="120"/>
-      <c r="F2" s="118" t="s">
+      <c r="C2" s="121"/>
+      <c r="D2" s="122"/>
+      <c r="F2" s="120" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="119"/>
-      <c r="H2" s="120"/>
-      <c r="J2" s="118" t="s">
+      <c r="G2" s="121"/>
+      <c r="H2" s="122"/>
+      <c r="J2" s="120" t="s">
         <v>92</v>
       </c>
-      <c r="K2" s="119"/>
-      <c r="L2" s="120"/>
-      <c r="N2" s="118" t="s">
+      <c r="K2" s="121"/>
+      <c r="L2" s="122"/>
+      <c r="N2" s="120" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="119"/>
-      <c r="P2" s="120"/>
-      <c r="R2" s="118" t="s">
+      <c r="O2" s="121"/>
+      <c r="P2" s="122"/>
+      <c r="R2" s="120" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="119"/>
-      <c r="T2" s="120"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="122"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="114" t="s">
+      <c r="C4" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="114"/>
-      <c r="F4" s="121" t="s">
+      <c r="D4" s="103"/>
+      <c r="F4" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="114" t="s">
+      <c r="G4" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="114"/>
-      <c r="J4" s="121" t="s">
+      <c r="H4" s="103"/>
+      <c r="J4" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="114" t="s">
+      <c r="K4" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="114"/>
-      <c r="N4" s="121" t="s">
+      <c r="L4" s="103"/>
+      <c r="N4" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="O4" s="114" t="s">
+      <c r="O4" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="114"/>
-      <c r="R4" s="121" t="s">
+      <c r="P4" s="103"/>
+      <c r="R4" s="123" t="s">
         <v>68</v>
       </c>
-      <c r="S4" s="114" t="s">
+      <c r="S4" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="T4" s="114"/>
+      <c r="T4" s="103"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="121"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="123"/>
+      <c r="C5" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F5" s="121"/>
-      <c r="G5" s="32" t="s">
+      <c r="F5" s="123"/>
+      <c r="G5" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="44">
+      <c r="H5" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J5" s="121"/>
-      <c r="K5" s="32" t="s">
+      <c r="J5" s="123"/>
+      <c r="K5" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="44">
+      <c r="L5" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N5" s="121"/>
-      <c r="O5" s="32" t="s">
+      <c r="N5" s="123"/>
+      <c r="O5" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="P5" s="44">
+      <c r="P5" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="R5" s="121"/>
-      <c r="S5" s="32" t="s">
+      <c r="R5" s="123"/>
+      <c r="S5" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="T5" s="44">
+      <c r="T5" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="121"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="123"/>
+      <c r="C6" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="43">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="F6" s="121"/>
-      <c r="G6" s="32" t="s">
+      <c r="F6" s="123"/>
+      <c r="G6" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="43">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="J6" s="121"/>
-      <c r="K6" s="32" t="s">
+      <c r="J6" s="123"/>
+      <c r="K6" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="44">
+      <c r="L6" s="43">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="N6" s="121"/>
-      <c r="O6" s="32" t="s">
+      <c r="N6" s="123"/>
+      <c r="O6" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="43">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
-      <c r="R6" s="121"/>
-      <c r="S6" s="32" t="s">
+      <c r="R6" s="123"/>
+      <c r="S6" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="T6" s="44">
+      <c r="T6" s="43">
         <f>40000/12</f>
         <v>3333.3333333333335</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="121"/>
-      <c r="C7" s="45" t="s">
+      <c r="B7" s="123"/>
+      <c r="C7" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="121"/>
-      <c r="G7" s="45" t="s">
+      <c r="F7" s="123"/>
+      <c r="G7" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="43">
         <f>12500+(H10*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="J7" s="121"/>
-      <c r="K7" s="45" t="s">
+      <c r="J7" s="123"/>
+      <c r="K7" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="L7" s="44">
+      <c r="L7" s="43">
         <f>12500+(L10*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="N7" s="121"/>
-      <c r="O7" s="45" t="s">
+      <c r="N7" s="123"/>
+      <c r="O7" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="P7" s="44">
+      <c r="P7" s="43">
         <f>12500+(P10*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="R7" s="121"/>
-      <c r="S7" s="45" t="s">
+      <c r="R7" s="123"/>
+      <c r="S7" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="T7" s="44">
+      <c r="T7" s="43">
         <f>12500+(T10*0.1)</f>
         <v>13062.4</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="121"/>
-      <c r="C8" s="114" t="s">
+      <c r="B8" s="123"/>
+      <c r="C8" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="114"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="114" t="s">
+      <c r="D8" s="103"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="H8" s="114"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="114" t="s">
+      <c r="H8" s="103"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="L8" s="114"/>
-      <c r="N8" s="121"/>
-      <c r="O8" s="114" t="s">
+      <c r="L8" s="103"/>
+      <c r="N8" s="123"/>
+      <c r="O8" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="P8" s="114"/>
-      <c r="R8" s="121"/>
-      <c r="S8" s="114" t="s">
+      <c r="P8" s="103"/>
+      <c r="R8" s="123"/>
+      <c r="S8" s="103" t="s">
         <v>77</v>
       </c>
-      <c r="T8" s="114"/>
+      <c r="T8" s="103"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="121"/>
-      <c r="C9" s="50" t="s">
+      <c r="B9" s="123"/>
+      <c r="C9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="121"/>
-      <c r="G9" s="32" t="s">
+      <c r="F9" s="123"/>
+      <c r="G9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="43">
         <f>SUM(D33+D34)</f>
         <v>16871.999999999996</v>
       </c>
-      <c r="J9" s="121"/>
-      <c r="K9" s="32" t="s">
+      <c r="J9" s="123"/>
+      <c r="K9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="44">
+      <c r="L9" s="43">
         <f>SUM(H33+H34)</f>
         <v>39367.999999999993</v>
       </c>
-      <c r="N9" s="121"/>
-      <c r="O9" s="32" t="s">
+      <c r="N9" s="123"/>
+      <c r="O9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="P9" s="44">
+      <c r="P9" s="43">
         <f>SUM(L33+L34)</f>
         <v>61863.999999999993</v>
       </c>
-      <c r="R9" s="121"/>
-      <c r="S9" s="32" t="s">
+      <c r="R9" s="123"/>
+      <c r="S9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="T9" s="44">
+      <c r="T9" s="43">
         <f>SUM(P33+P34)</f>
         <v>84359.999999999985</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="121"/>
-      <c r="C10" s="52" t="s">
+      <c r="B10" s="123"/>
+      <c r="C10" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="121"/>
-      <c r="G10" s="32" t="s">
+      <c r="F10" s="123"/>
+      <c r="G10" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J10" s="121"/>
-      <c r="K10" s="32" t="s">
+      <c r="J10" s="123"/>
+      <c r="K10" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="44">
+      <c r="L10" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N10" s="121"/>
-      <c r="O10" s="32" t="s">
+      <c r="N10" s="123"/>
+      <c r="O10" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="P10" s="44">
+      <c r="P10" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="R10" s="121"/>
-      <c r="S10" s="32" t="s">
+      <c r="R10" s="123"/>
+      <c r="S10" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="T10" s="44">
+      <c r="T10" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="49"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="49"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="49"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="47"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="47"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="47"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="46"/>
+      <c r="T11" s="47"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="114" t="s">
+      <c r="C12" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="114"/>
-      <c r="F12" s="105" t="s">
+      <c r="D12" s="103"/>
+      <c r="F12" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="114" t="s">
+      <c r="G12" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="114"/>
-      <c r="J12" s="105" t="s">
+      <c r="H12" s="103"/>
+      <c r="J12" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="114" t="s">
+      <c r="K12" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="114"/>
-      <c r="N12" s="105" t="s">
+      <c r="L12" s="103"/>
+      <c r="N12" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="O12" s="114" t="s">
+      <c r="O12" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="P12" s="114"/>
-      <c r="R12" s="105" t="s">
+      <c r="P12" s="103"/>
+      <c r="R12" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="S12" s="114" t="s">
+      <c r="S12" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="T12" s="114"/>
+      <c r="T12" s="103"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="106"/>
-      <c r="C13" s="32" t="s">
+      <c r="B13" s="107"/>
+      <c r="C13" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F13" s="106"/>
-      <c r="G13" s="32" t="s">
+      <c r="F13" s="107"/>
+      <c r="G13" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J13" s="106"/>
-      <c r="K13" s="32" t="s">
+      <c r="J13" s="107"/>
+      <c r="K13" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="L13" s="44">
+      <c r="L13" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N13" s="106"/>
-      <c r="O13" s="32" t="s">
+      <c r="N13" s="107"/>
+      <c r="O13" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="P13" s="44">
+      <c r="P13" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="R13" s="106"/>
-      <c r="S13" s="32" t="s">
+      <c r="R13" s="107"/>
+      <c r="S13" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="T13" s="44">
+      <c r="T13" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="106"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="107"/>
+      <c r="C14" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="43">
         <v>10000</v>
       </c>
-      <c r="F14" s="106"/>
-      <c r="G14" s="32" t="s">
+      <c r="F14" s="107"/>
+      <c r="G14" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="44">
+      <c r="H14" s="43">
         <v>10000</v>
       </c>
-      <c r="J14" s="106"/>
-      <c r="K14" s="32" t="s">
+      <c r="J14" s="107"/>
+      <c r="K14" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="L14" s="44">
+      <c r="L14" s="43">
         <v>10000</v>
       </c>
-      <c r="N14" s="106"/>
-      <c r="O14" s="32" t="s">
+      <c r="N14" s="107"/>
+      <c r="O14" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="P14" s="44">
+      <c r="P14" s="43">
         <v>10000</v>
       </c>
-      <c r="R14" s="106"/>
-      <c r="S14" s="32" t="s">
+      <c r="R14" s="107"/>
+      <c r="S14" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="T14" s="44">
+      <c r="T14" s="43">
         <v>10000</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="106"/>
-      <c r="C15" s="45" t="s">
+      <c r="B15" s="107"/>
+      <c r="C15" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="43">
         <f>12500+(D18*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="F15" s="106"/>
-      <c r="G15" s="45" t="s">
+      <c r="F15" s="107"/>
+      <c r="G15" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="43">
         <f>12500+(H18*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="J15" s="106"/>
-      <c r="K15" s="45" t="s">
+      <c r="J15" s="107"/>
+      <c r="K15" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="44">
+      <c r="L15" s="43">
         <f>12500+(L18*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="N15" s="106"/>
-      <c r="O15" s="45" t="s">
+      <c r="N15" s="107"/>
+      <c r="O15" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="43">
         <f>12500+(P18*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="R15" s="106"/>
-      <c r="S15" s="45" t="s">
+      <c r="R15" s="107"/>
+      <c r="S15" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="T15" s="44">
+      <c r="T15" s="43">
         <f>12500+(T18*0.1)</f>
         <v>13062.4</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="106"/>
-      <c r="C16" s="114" t="s">
+      <c r="B16" s="107"/>
+      <c r="C16" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="114"/>
-      <c r="F16" s="106"/>
-      <c r="G16" s="114" t="s">
+      <c r="D16" s="103"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="114"/>
-      <c r="J16" s="106"/>
-      <c r="K16" s="114" t="s">
+      <c r="H16" s="103"/>
+      <c r="J16" s="107"/>
+      <c r="K16" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="L16" s="114"/>
-      <c r="N16" s="106"/>
-      <c r="O16" s="114" t="s">
+      <c r="L16" s="103"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="P16" s="114"/>
-      <c r="R16" s="106"/>
-      <c r="S16" s="114" t="s">
+      <c r="P16" s="103"/>
+      <c r="R16" s="107"/>
+      <c r="S16" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="T16" s="114"/>
+      <c r="T16" s="103"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="106"/>
-      <c r="C17" s="50" t="s">
+      <c r="B17" s="107"/>
+      <c r="C17" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="106"/>
-      <c r="G17" s="32" t="s">
+      <c r="F17" s="107"/>
+      <c r="G17" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="51">
         <f>SUM(H9:H10)</f>
         <v>22495.999999999996</v>
       </c>
-      <c r="J17" s="106"/>
-      <c r="K17" s="32" t="s">
+      <c r="J17" s="107"/>
+      <c r="K17" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="L17" s="54">
+      <c r="L17" s="51">
         <f>SUM(L9:L10)</f>
         <v>44991.999999999993</v>
       </c>
-      <c r="N17" s="106"/>
-      <c r="O17" s="32" t="s">
+      <c r="N17" s="107"/>
+      <c r="O17" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="P17" s="54">
+      <c r="P17" s="51">
         <f>SUM(P9:P10)</f>
         <v>67487.999999999985</v>
       </c>
-      <c r="R17" s="106"/>
-      <c r="S17" s="32" t="s">
+      <c r="R17" s="107"/>
+      <c r="S17" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="T17" s="54">
+      <c r="T17" s="51">
         <f>SUM(T9:T10)</f>
         <v>89983.999999999985</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="107"/>
-      <c r="C18" s="32" t="s">
+      <c r="B18" s="108"/>
+      <c r="C18" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="44">
+      <c r="D18" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F18" s="107"/>
-      <c r="G18" s="32" t="s">
+      <c r="F18" s="108"/>
+      <c r="G18" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J18" s="107"/>
-      <c r="K18" s="32" t="s">
+      <c r="J18" s="108"/>
+      <c r="K18" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="L18" s="44">
+      <c r="L18" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N18" s="107"/>
-      <c r="O18" s="32" t="s">
+      <c r="N18" s="108"/>
+      <c r="O18" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="R18" s="107"/>
-      <c r="S18" s="32" t="s">
+      <c r="R18" s="108"/>
+      <c r="S18" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="T18" s="44">
+      <c r="T18" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="H19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="T19" s="43"/>
+      <c r="H19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="T19" s="42"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="117" t="s">
+      <c r="B20" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="114" t="s">
+      <c r="C20" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="114"/>
-      <c r="F20" s="117" t="s">
+      <c r="D20" s="103"/>
+      <c r="F20" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="G20" s="114" t="s">
+      <c r="G20" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="114"/>
-      <c r="J20" s="117" t="s">
+      <c r="H20" s="103"/>
+      <c r="J20" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="K20" s="114" t="s">
+      <c r="K20" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="L20" s="114"/>
-      <c r="N20" s="117" t="s">
+      <c r="L20" s="103"/>
+      <c r="N20" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="O20" s="114" t="s">
+      <c r="O20" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="P20" s="114"/>
-      <c r="R20" s="117" t="s">
+      <c r="P20" s="103"/>
+      <c r="R20" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="S20" s="114" t="s">
+      <c r="S20" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="T20" s="114"/>
+      <c r="T20" s="103"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="117"/>
-      <c r="C21" s="32" t="s">
+      <c r="B21" s="119"/>
+      <c r="C21" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="44">
+      <c r="D21" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F21" s="117"/>
-      <c r="G21" s="32" t="s">
+      <c r="F21" s="119"/>
+      <c r="G21" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="44">
+      <c r="H21" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J21" s="117"/>
-      <c r="K21" s="32" t="s">
+      <c r="J21" s="119"/>
+      <c r="K21" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="L21" s="44">
+      <c r="L21" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N21" s="117"/>
-      <c r="O21" s="32" t="s">
+      <c r="N21" s="119"/>
+      <c r="O21" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="P21" s="44">
+      <c r="P21" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="R21" s="117"/>
-      <c r="S21" s="32" t="s">
+      <c r="R21" s="119"/>
+      <c r="S21" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="T21" s="44">
+      <c r="T21" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="117"/>
-      <c r="C22" s="32" t="s">
+      <c r="B22" s="119"/>
+      <c r="C22" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="44">
+      <c r="D22" s="43">
         <v>10000</v>
       </c>
-      <c r="F22" s="117"/>
-      <c r="G22" s="32" t="s">
+      <c r="F22" s="119"/>
+      <c r="G22" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="44">
+      <c r="H22" s="43">
         <v>10000</v>
       </c>
-      <c r="J22" s="117"/>
-      <c r="K22" s="32" t="s">
+      <c r="J22" s="119"/>
+      <c r="K22" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="L22" s="44">
+      <c r="L22" s="43">
         <v>10000</v>
       </c>
-      <c r="N22" s="117"/>
-      <c r="O22" s="32" t="s">
+      <c r="N22" s="119"/>
+      <c r="O22" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="P22" s="44">
+      <c r="P22" s="43">
         <v>10000</v>
       </c>
-      <c r="R22" s="117"/>
-      <c r="S22" s="32" t="s">
+      <c r="R22" s="119"/>
+      <c r="S22" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="T22" s="44">
+      <c r="T22" s="43">
         <v>10000</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="117"/>
-      <c r="C23" s="45" t="s">
+      <c r="B23" s="119"/>
+      <c r="C23" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="44">
+      <c r="D23" s="43">
         <f>12500+(D25*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="F23" s="117"/>
-      <c r="G23" s="45" t="s">
+      <c r="F23" s="119"/>
+      <c r="G23" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="H23" s="44">
+      <c r="H23" s="43">
         <f>12500+(H26*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="J23" s="117"/>
-      <c r="K23" s="45" t="s">
+      <c r="J23" s="119"/>
+      <c r="K23" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="L23" s="44">
+      <c r="L23" s="43">
         <f>12500+(L26*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="N23" s="117"/>
-      <c r="O23" s="45" t="s">
+      <c r="N23" s="119"/>
+      <c r="O23" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="P23" s="44">
+      <c r="P23" s="43">
         <f>12500+(P26*0.1)</f>
         <v>13062.4</v>
       </c>
-      <c r="R23" s="117"/>
-      <c r="S23" s="45" t="s">
+      <c r="R23" s="119"/>
+      <c r="S23" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="T23" s="44">
+      <c r="T23" s="43">
         <f>12500+(T26*0.1)</f>
         <v>13062.4</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="117"/>
-      <c r="C24" s="114" t="s">
+      <c r="B24" s="119"/>
+      <c r="C24" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="114"/>
-      <c r="F24" s="117"/>
-      <c r="G24" s="114" t="s">
+      <c r="D24" s="103"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="H24" s="114"/>
-      <c r="J24" s="117"/>
-      <c r="K24" s="114" t="s">
+      <c r="H24" s="103"/>
+      <c r="J24" s="119"/>
+      <c r="K24" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="L24" s="114"/>
-      <c r="N24" s="117"/>
-      <c r="O24" s="114" t="s">
+      <c r="L24" s="103"/>
+      <c r="N24" s="119"/>
+      <c r="O24" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="P24" s="114"/>
-      <c r="R24" s="117"/>
-      <c r="S24" s="114" t="s">
+      <c r="P24" s="103"/>
+      <c r="R24" s="119"/>
+      <c r="S24" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="T24" s="114"/>
+      <c r="T24" s="103"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="117"/>
-      <c r="C25" s="32" t="s">
+      <c r="B25" s="119"/>
+      <c r="C25" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="44">
+      <c r="D25" s="43">
         <f>D18</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F25" s="117"/>
-      <c r="G25" s="32" t="s">
+      <c r="F25" s="119"/>
+      <c r="G25" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="43">
         <f>SUM(H17:H18)</f>
         <v>28119.999999999996</v>
       </c>
-      <c r="J25" s="117"/>
-      <c r="K25" s="32" t="s">
+      <c r="J25" s="119"/>
+      <c r="K25" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="L25" s="44">
+      <c r="L25" s="43">
         <f>SUM(L17:L18)</f>
         <v>50615.999999999993</v>
       </c>
-      <c r="N25" s="117"/>
-      <c r="O25" s="32" t="s">
+      <c r="N25" s="119"/>
+      <c r="O25" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="P25" s="44">
+      <c r="P25" s="43">
         <f>SUM(P17:P18)</f>
         <v>73111.999999999985</v>
       </c>
-      <c r="R25" s="117"/>
-      <c r="S25" s="32" t="s">
+      <c r="R25" s="119"/>
+      <c r="S25" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="T25" s="44">
+      <c r="T25" s="43">
         <f>SUM(T17:T18)</f>
         <v>95607.999999999985</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="117"/>
-      <c r="C26" s="32" t="s">
+      <c r="B26" s="119"/>
+      <c r="C26" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="44">
+      <c r="D26" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F26" s="117"/>
-      <c r="G26" s="32" t="s">
+      <c r="F26" s="119"/>
+      <c r="G26" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="44">
+      <c r="H26" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J26" s="117"/>
-      <c r="K26" s="32" t="s">
+      <c r="J26" s="119"/>
+      <c r="K26" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L26" s="44">
+      <c r="L26" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N26" s="117"/>
-      <c r="O26" s="32" t="s">
+      <c r="N26" s="119"/>
+      <c r="O26" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="P26" s="44">
+      <c r="P26" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="R26" s="117"/>
-      <c r="S26" s="32" t="s">
+      <c r="R26" s="119"/>
+      <c r="S26" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="T26" s="44">
+      <c r="T26" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="H27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="T27" s="43"/>
+      <c r="H27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="T27" s="42"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="114" t="s">
+      <c r="C28" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="114"/>
-      <c r="F28" s="117" t="s">
+      <c r="D28" s="103"/>
+      <c r="F28" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="G28" s="114" t="s">
+      <c r="G28" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="H28" s="114"/>
-      <c r="J28" s="117" t="s">
+      <c r="H28" s="103"/>
+      <c r="J28" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="K28" s="114" t="s">
+      <c r="K28" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="L28" s="114"/>
-      <c r="N28" s="117" t="s">
+      <c r="L28" s="103"/>
+      <c r="N28" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="O28" s="114" t="s">
+      <c r="O28" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="P28" s="114"/>
-      <c r="R28" s="117" t="s">
+      <c r="P28" s="103"/>
+      <c r="R28" s="119" t="s">
         <v>85</v>
       </c>
-      <c r="S28" s="114" t="s">
+      <c r="S28" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="T28" s="114"/>
+      <c r="T28" s="103"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="117"/>
-      <c r="C29" s="32" t="s">
+      <c r="B29" s="119"/>
+      <c r="C29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="44">
+      <c r="D29" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="F29" s="117"/>
-      <c r="G29" s="32" t="s">
+      <c r="F29" s="119"/>
+      <c r="G29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="44">
+      <c r="H29" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="J29" s="117"/>
-      <c r="K29" s="32" t="s">
+      <c r="J29" s="119"/>
+      <c r="K29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="L29" s="44">
+      <c r="L29" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="N29" s="117"/>
-      <c r="O29" s="32" t="s">
+      <c r="N29" s="119"/>
+      <c r="O29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="P29" s="44">
+      <c r="P29" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
-      <c r="R29" s="117"/>
-      <c r="S29" s="32" t="s">
+      <c r="R29" s="119"/>
+      <c r="S29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="T29" s="44">
+      <c r="T29" s="43">
         <f>'Required sales'!$E$5*3</f>
         <v>23750</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="117"/>
-      <c r="C30" s="32" t="s">
+      <c r="B30" s="119"/>
+      <c r="C30" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="44">
+      <c r="D30" s="43">
         <v>10000</v>
       </c>
-      <c r="F30" s="117"/>
-      <c r="G30" s="32" t="s">
+      <c r="F30" s="119"/>
+      <c r="G30" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="H30" s="44">
+      <c r="H30" s="43">
         <v>10000</v>
       </c>
-      <c r="J30" s="117"/>
-      <c r="K30" s="32" t="s">
+      <c r="J30" s="119"/>
+      <c r="K30" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="L30" s="44">
+      <c r="L30" s="43">
         <v>10000</v>
       </c>
-      <c r="N30" s="117"/>
-      <c r="O30" s="32" t="s">
+      <c r="N30" s="119"/>
+      <c r="O30" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="P30" s="44">
+      <c r="P30" s="43">
         <v>10000</v>
       </c>
-      <c r="R30" s="117"/>
-      <c r="S30" s="32" t="s">
+      <c r="R30" s="119"/>
+      <c r="S30" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="T30" s="44">
+      <c r="T30" s="43">
         <v>10000</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="117"/>
-      <c r="C31" s="45" t="s">
+      <c r="B31" s="119"/>
+      <c r="C31" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="44">
+      <c r="D31" s="43">
         <f>12500+(D33*0.1)</f>
         <v>13624.8</v>
       </c>
-      <c r="F31" s="117"/>
-      <c r="G31" s="45" t="s">
+      <c r="F31" s="119"/>
+      <c r="G31" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="44">
+      <c r="H31" s="43">
         <f>12500+(H33*0.1)</f>
         <v>15874.4</v>
       </c>
-      <c r="J31" s="117"/>
-      <c r="K31" s="45" t="s">
+      <c r="J31" s="119"/>
+      <c r="K31" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="L31" s="44">
+      <c r="L31" s="43">
         <f>12500+(L33*0.1)</f>
         <v>18124</v>
       </c>
-      <c r="N31" s="117"/>
-      <c r="O31" s="45" t="s">
+      <c r="N31" s="119"/>
+      <c r="O31" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="P31" s="44">
+      <c r="P31" s="43">
         <f>12500+(P33*0.1)</f>
         <v>20373.599999999999</v>
       </c>
-      <c r="R31" s="117"/>
-      <c r="S31" s="45" t="s">
+      <c r="R31" s="119"/>
+      <c r="S31" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="T31" s="44">
+      <c r="T31" s="43">
         <f>12500+(T33*0.1)</f>
         <v>22623.199999999997</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="117"/>
-      <c r="C32" s="114" t="s">
+      <c r="B32" s="119"/>
+      <c r="C32" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="114"/>
-      <c r="F32" s="117"/>
-      <c r="G32" s="114" t="s">
+      <c r="D32" s="103"/>
+      <c r="F32" s="119"/>
+      <c r="G32" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="114"/>
-      <c r="J32" s="117"/>
-      <c r="K32" s="114" t="s">
+      <c r="H32" s="103"/>
+      <c r="J32" s="119"/>
+      <c r="K32" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="L32" s="114"/>
-      <c r="N32" s="117"/>
-      <c r="O32" s="114" t="s">
+      <c r="L32" s="103"/>
+      <c r="N32" s="119"/>
+      <c r="O32" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="P32" s="114"/>
-      <c r="R32" s="117"/>
-      <c r="S32" s="114" t="s">
+      <c r="P32" s="103"/>
+      <c r="R32" s="119"/>
+      <c r="S32" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="T32" s="114"/>
+      <c r="T32" s="103"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="117"/>
-      <c r="C33" s="32" t="s">
+      <c r="B33" s="119"/>
+      <c r="C33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="44">
+      <c r="D33" s="43">
         <f>D25+D26</f>
         <v>11247.999999999998</v>
       </c>
-      <c r="F33" s="117"/>
-      <c r="G33" s="32" t="s">
+      <c r="F33" s="119"/>
+      <c r="G33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="H33" s="44">
+      <c r="H33" s="43">
         <f>H25+H26</f>
         <v>33743.999999999993</v>
       </c>
-      <c r="J33" s="117"/>
-      <c r="K33" s="32" t="s">
+      <c r="J33" s="119"/>
+      <c r="K33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="L33" s="44">
+      <c r="L33" s="43">
         <f>L25+L26</f>
         <v>56239.999999999993</v>
       </c>
-      <c r="N33" s="117"/>
-      <c r="O33" s="32" t="s">
+      <c r="N33" s="119"/>
+      <c r="O33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="P33" s="44">
+      <c r="P33" s="43">
         <f>P25+P26</f>
         <v>78735.999999999985</v>
       </c>
-      <c r="R33" s="117"/>
-      <c r="S33" s="32" t="s">
+      <c r="R33" s="119"/>
+      <c r="S33" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="T33" s="44">
+      <c r="T33" s="43">
         <f>T25+T26</f>
         <v>101231.99999999999</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="117"/>
-      <c r="C34" s="32" t="s">
+      <c r="B34" s="119"/>
+      <c r="C34" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="44">
+      <c r="D34" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="F34" s="117"/>
-      <c r="G34" s="32" t="s">
+      <c r="F34" s="119"/>
+      <c r="G34" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="H34" s="44">
+      <c r="H34" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="J34" s="117"/>
-      <c r="K34" s="32" t="s">
+      <c r="J34" s="119"/>
+      <c r="K34" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="L34" s="44">
+      <c r="L34" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="N34" s="117"/>
-      <c r="O34" s="32" t="s">
+      <c r="N34" s="119"/>
+      <c r="O34" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="P34" s="44">
+      <c r="P34" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
-      <c r="R34" s="117"/>
-      <c r="S34" s="32" t="s">
+      <c r="R34" s="119"/>
+      <c r="S34" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="T34" s="44">
+      <c r="T34" s="43">
         <f>'Required sales'!$E$11/3</f>
         <v>5623.9999999999991</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="H35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="T35" s="43"/>
+      <c r="H35" s="42"/>
+      <c r="L35" s="42"/>
+      <c r="P35" s="42"/>
+      <c r="T35" s="42"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="115" t="s">
+      <c r="B36" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="115"/>
-      <c r="D36" s="44">
+      <c r="C36" s="117"/>
+      <c r="D36" s="43">
         <f>SUM(D18,D25:D26,D33:D34)</f>
         <v>33743.999999999993</v>
       </c>
-      <c r="F36" s="115" t="s">
+      <c r="F36" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="G36" s="115"/>
-      <c r="H36" s="44">
+      <c r="G36" s="117"/>
+      <c r="H36" s="43">
         <f>SUM(H9:H10,H17:H18,H25:H26,H33:H34)</f>
         <v>123727.99999999997</v>
       </c>
-      <c r="J36" s="115" t="s">
+      <c r="J36" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="K36" s="115"/>
-      <c r="L36" s="44">
+      <c r="K36" s="117"/>
+      <c r="L36" s="43">
         <f>SUM(L9:L10,L17:L18,L25:L26,L33:L34)</f>
         <v>213711.99999999997</v>
       </c>
-      <c r="N36" s="115" t="s">
+      <c r="N36" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="O36" s="115"/>
-      <c r="P36" s="44">
+      <c r="O36" s="117"/>
+      <c r="P36" s="43">
         <f>SUM(P9:P10,P17:P18,P25:P26,P33:P34)</f>
         <v>303695.99999999994</v>
       </c>
-      <c r="R36" s="115" t="s">
+      <c r="R36" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="S36" s="115"/>
-      <c r="T36" s="44">
+      <c r="S36" s="117"/>
+      <c r="T36" s="43">
         <f>SUM(T9:T10,T17:T18,T25:T26,T33:T34)</f>
         <v>393679.99999999994</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="115" t="s">
+      <c r="B37" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="115"/>
-      <c r="D37" s="44">
+      <c r="C37" s="117"/>
+      <c r="D37" s="43">
         <f>SUM(D5:D6,D13:D15,D21:D23,D29:D31)</f>
         <v>168082.93333333329</v>
       </c>
-      <c r="F37" s="115" t="s">
+      <c r="F37" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="G37" s="115"/>
-      <c r="H37" s="44">
+      <c r="G37" s="117"/>
+      <c r="H37" s="43">
         <f>SUM(H5:H6,H13:H15,H21:H23,H29:H31)</f>
         <v>170332.5333333333</v>
       </c>
-      <c r="J37" s="115" t="s">
+      <c r="J37" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="K37" s="115"/>
-      <c r="L37" s="44">
+      <c r="K37" s="117"/>
+      <c r="L37" s="43">
         <f>SUM(L5:L6,L13:L15,L21:L23,L29:L31)</f>
         <v>172582.1333333333</v>
       </c>
-      <c r="N37" s="115" t="s">
+      <c r="N37" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="O37" s="115"/>
-      <c r="P37" s="44">
+      <c r="O37" s="117"/>
+      <c r="P37" s="43">
         <f>SUM(P5:P6,P13:P15,P21:P23,P29:P31)</f>
         <v>174831.73333333331</v>
       </c>
-      <c r="R37" s="115" t="s">
+      <c r="R37" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="S37" s="115"/>
-      <c r="T37" s="44">
+      <c r="S37" s="117"/>
+      <c r="T37" s="43">
         <f>SUM(T5:T6,T13:T15,T21:T23,T29:T31)</f>
         <v>177081.33333333331</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="H38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="P38" s="43"/>
-      <c r="T38" s="43"/>
+      <c r="H38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="P38" s="42"/>
+      <c r="T38" s="42"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="116"/>
-      <c r="D39" s="44">
+      <c r="C39" s="118"/>
+      <c r="D39" s="43">
         <f>0-D37+D36</f>
         <v>-134338.93333333329</v>
       </c>
-      <c r="F39" s="116" t="s">
+      <c r="F39" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="G39" s="116"/>
-      <c r="H39" s="44">
+      <c r="G39" s="118"/>
+      <c r="H39" s="43">
         <f>0-H37+H36</f>
         <v>-46604.533333333326</v>
       </c>
-      <c r="J39" s="116" t="s">
+      <c r="J39" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="K39" s="116"/>
-      <c r="L39" s="44">
+      <c r="K39" s="118"/>
+      <c r="L39" s="43">
         <f>0-L37+L36</f>
         <v>41129.866666666669</v>
       </c>
-      <c r="N39" s="116" t="s">
+      <c r="N39" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="O39" s="116"/>
-      <c r="P39" s="44">
+      <c r="O39" s="118"/>
+      <c r="P39" s="43">
         <f>0-P37+P36</f>
         <v>128864.26666666663</v>
       </c>
-      <c r="R39" s="116" t="s">
+      <c r="R39" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="S39" s="116"/>
-      <c r="T39" s="44">
+      <c r="S39" s="118"/>
+      <c r="T39" s="43">
         <f>0-T37+T36</f>
         <v>216598.66666666663</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B40" s="116" t="s">
+      <c r="B40" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="116"/>
-      <c r="D40" s="44">
+      <c r="C40" s="118"/>
+      <c r="D40" s="43">
         <f>D39</f>
         <v>-134338.93333333329</v>
       </c>
-      <c r="F40" s="116" t="s">
+      <c r="F40" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="G40" s="116"/>
-      <c r="H40" s="44">
+      <c r="G40" s="118"/>
+      <c r="H40" s="43">
         <f>D40+H39</f>
         <v>-180943.46666666662</v>
       </c>
-      <c r="J40" s="116" t="s">
+      <c r="J40" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="K40" s="116"/>
-      <c r="L40" s="44">
+      <c r="K40" s="118"/>
+      <c r="L40" s="43">
         <f>H40+L39</f>
         <v>-139813.59999999995</v>
       </c>
-      <c r="N40" s="116" t="s">
+      <c r="N40" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="O40" s="116"/>
-      <c r="P40" s="44">
+      <c r="O40" s="118"/>
+      <c r="P40" s="43">
         <f>L40+P39</f>
         <v>-10949.333333333314</v>
       </c>
-      <c r="R40" s="116" t="s">
+      <c r="R40" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="S40" s="116"/>
-      <c r="T40" s="44">
+      <c r="S40" s="118"/>
+      <c r="T40" s="43">
         <f>P40+T39</f>
         <v>205649.33333333331</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="116" t="s">
+      <c r="B42" s="118" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="116"/>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
-      <c r="F42" s="116"/>
-      <c r="G42" s="116"/>
-      <c r="H42" s="116"/>
-      <c r="I42" s="116"/>
-      <c r="J42" s="116"/>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-      <c r="O42" s="116"/>
-      <c r="P42" s="116"/>
-      <c r="Q42" s="116"/>
-      <c r="R42" s="116"/>
-      <c r="S42" s="116"/>
-      <c r="T42" s="116"/>
+      <c r="C42" s="118"/>
+      <c r="D42" s="118"/>
+      <c r="E42" s="118"/>
+      <c r="F42" s="118"/>
+      <c r="G42" s="118"/>
+      <c r="H42" s="118"/>
+      <c r="I42" s="118"/>
+      <c r="J42" s="118"/>
+      <c r="K42" s="118"/>
+      <c r="L42" s="118"/>
+      <c r="M42" s="118"/>
+      <c r="N42" s="118"/>
+      <c r="O42" s="118"/>
+      <c r="P42" s="118"/>
+      <c r="Q42" s="118"/>
+      <c r="R42" s="118"/>
+      <c r="S42" s="118"/>
+      <c r="T42" s="118"/>
     </row>
     <row r="43" spans="2:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="122" t="s">
+      <c r="B43" s="124" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="122"/>
-      <c r="D43" s="122"/>
-      <c r="E43" s="122"/>
-      <c r="F43" s="122"/>
-      <c r="G43" s="122"/>
-      <c r="H43" s="122"/>
-      <c r="I43" s="122"/>
-      <c r="J43" s="122"/>
-      <c r="K43" s="122"/>
-      <c r="L43" s="122"/>
-      <c r="M43" s="122"/>
-      <c r="N43" s="122"/>
-      <c r="O43" s="122"/>
-      <c r="P43" s="122"/>
-      <c r="Q43" s="122"/>
-      <c r="R43" s="122"/>
-      <c r="S43" s="122"/>
-      <c r="T43" s="122"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
+      <c r="E43" s="124"/>
+      <c r="F43" s="124"/>
+      <c r="G43" s="124"/>
+      <c r="H43" s="124"/>
+      <c r="I43" s="124"/>
+      <c r="J43" s="124"/>
+      <c r="K43" s="124"/>
+      <c r="L43" s="124"/>
+      <c r="M43" s="124"/>
+      <c r="N43" s="124"/>
+      <c r="O43" s="124"/>
+      <c r="P43" s="124"/>
+      <c r="Q43" s="124"/>
+      <c r="R43" s="124"/>
+      <c r="S43" s="124"/>
+      <c r="T43" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="R39:S39"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="B42:T42"/>
-    <mergeCell ref="R20:R26"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="R28:R34"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S32:T32"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R4:R10"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="R12:R18"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N20:N26"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="N28:N34"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N4:N10"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="N12:N18"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="J20:J26"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="J12:J18"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="F4:F10"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J4:J10"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="B43:T43"/>
     <mergeCell ref="F12:F18"/>
     <mergeCell ref="G12:H12"/>
@@ -4666,29 +4629,35 @@
     <mergeCell ref="F28:F34"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="F4:F10"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J4:J10"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="J28:J34"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R4:R10"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="R12:R18"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="R20:R26"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="R28:R34"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S32:T32"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="R39:S39"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="B42:T42"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="F37:G37"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="J20:J26"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="J12:J18"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="J37:K37"/>
     <mergeCell ref="J39:K39"/>
@@ -4698,30 +4667,12 @@
     <mergeCell ref="F39:G39"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N4:N10"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="N12:N18"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="N20:N26"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="N28:N34"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O32:P32"/>
   </mergeCells>
   <conditionalFormatting sqref="D39:D40">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>